<commit_message>
Changed version number formatting.
</commit_message>
<xml_diff>
--- a/dokumentation/tidsplan/tidsplan_v1.0.xlsx
+++ b/dokumentation/tidsplan/tidsplan_v1.0.xlsx
@@ -951,6 +951,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10.0"/>
@@ -1246,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
       <alignment/>
@@ -1274,6 +1277,9 @@
     </xf>
     <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="164" borderId="1" applyFont="1" fontId="4" applyNumberFormat="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf applyBorder="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4"/>
     <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
@@ -1496,12 +1502,12 @@
       <c t="s" s="7" r="G3">
         <v>7</v>
       </c>
-      <c s="8" r="I3">
+      <c s="10" r="I3">
         <v>1.0</v>
       </c>
-      <c s="10" r="P3"/>
-      <c s="11" r="Q3"/>
-      <c s="11" r="U3"/>
+      <c s="11" r="P3"/>
+      <c s="12" r="Q3"/>
+      <c s="12" r="U3"/>
     </row>
     <row customHeight="1" r="4" ht="11.25">
       <c t="s" s="7" r="A4">
@@ -1516,3065 +1522,3065 @@
       <c t="s" s="9" r="I4">
         <v>11</v>
       </c>
-      <c s="10" r="P4"/>
-      <c s="10" r="Q4"/>
-      <c s="10" r="U4"/>
+      <c s="11" r="P4"/>
+      <c s="11" r="Q4"/>
+      <c s="11" r="U4"/>
     </row>
     <row customHeight="1" r="5" ht="12.75">
-      <c t="s" s="12" r="A5">
+      <c t="s" s="13" r="A5">
         <v>12</v>
       </c>
-      <c t="s" s="13" r="F5">
+      <c t="s" s="14" r="F5">
         <v>13</v>
       </c>
-      <c t="s" s="14" r="G5">
+      <c t="s" s="15" r="G5">
         <v>14</v>
       </c>
-      <c t="s" s="15" r="H5">
+      <c t="s" s="16" r="H5">
         <v>15</v>
       </c>
-      <c t="s" s="16" r="T5">
+      <c t="s" s="17" r="T5">
         <v>16</v>
       </c>
-      <c s="16" r="U5"/>
+      <c s="17" r="U5"/>
     </row>
     <row r="6">
-      <c t="s" s="17" r="A6">
+      <c t="s" s="18" r="A6">
         <v>17</v>
       </c>
-      <c t="s" s="18" r="B6">
+      <c t="s" s="19" r="B6">
         <v>18</v>
       </c>
-      <c t="s" s="19" r="E6">
+      <c t="s" s="20" r="E6">
         <v>19</v>
       </c>
-      <c t="s" s="20" r="F6">
+      <c t="s" s="21" r="F6">
         <v>20</v>
       </c>
-      <c t="s" s="21" r="G6">
+      <c t="s" s="22" r="G6">
         <v>21</v>
       </c>
-      <c s="20" r="H6">
+      <c s="21" r="H6">
         <v>40.0</v>
       </c>
-      <c s="21" r="I6">
+      <c s="22" r="I6">
         <v>41.0</v>
       </c>
-      <c s="21" r="J6">
+      <c s="22" r="J6">
         <v>42.0</v>
       </c>
-      <c s="21" r="K6">
+      <c s="22" r="K6">
         <v>43.0</v>
       </c>
-      <c s="21" r="L6">
+      <c s="22" r="L6">
         <v>44.0</v>
       </c>
-      <c s="21" r="M6">
+      <c s="22" r="M6">
         <v>45.0</v>
       </c>
-      <c s="21" r="N6">
+      <c s="22" r="N6">
         <v>46.0</v>
       </c>
-      <c s="21" r="O6">
+      <c s="22" r="O6">
         <v>47.0</v>
       </c>
-      <c s="20" r="P6">
+      <c s="21" r="P6">
         <v>48.0</v>
       </c>
-      <c s="21" r="Q6">
+      <c s="22" r="Q6">
         <v>49.0</v>
       </c>
-      <c s="21" r="R6">
+      <c s="22" r="R6">
         <v>50.0</v>
       </c>
-      <c s="22" r="S6">
+      <c s="23" r="S6">
         <v>51.0</v>
       </c>
-      <c s="23" r="T6"/>
-      <c s="23" r="U6"/>
+      <c s="24" r="T6"/>
+      <c s="24" r="U6"/>
     </row>
     <row r="7">
-      <c s="18" r="A7">
+      <c s="19" r="A7">
         <v>1.0</v>
       </c>
-      <c t="s" s="24" r="B7">
+      <c t="s" s="25" r="B7">
         <v>22</v>
       </c>
-      <c s="25" r="E7"/>
-      <c s="26" r="F7">
+      <c s="26" r="E7"/>
+      <c s="27" r="F7">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G7">
+      <c t="s" s="28" r="G7">
         <v>23</v>
       </c>
-      <c s="27" r="H7"/>
-      <c s="27" r="I7"/>
-      <c s="28" r="J7"/>
-      <c t="s" s="29" r="K7">
+      <c s="28" r="H7"/>
+      <c s="28" r="I7"/>
+      <c s="29" r="J7"/>
+      <c t="s" s="30" r="K7">
         <v>24</v>
       </c>
-      <c t="s" s="29" r="L7">
+      <c t="s" s="30" r="L7">
         <v>25</v>
       </c>
-      <c s="27" r="M7">
+      <c s="28" r="M7">
         <v>16.0</v>
       </c>
-      <c s="28" r="N7"/>
-      <c s="28" r="O7"/>
-      <c s="28" r="P7"/>
-      <c s="28" r="Q7"/>
-      <c s="28" r="R7"/>
-      <c s="28" r="S7"/>
-      <c t="str" s="30" r="T7">
+      <c s="29" r="N7"/>
+      <c s="29" r="O7"/>
+      <c s="29" r="P7"/>
+      <c s="29" r="Q7"/>
+      <c s="29" r="R7"/>
+      <c s="29" r="S7"/>
+      <c t="str" s="31" r="T7">
         <f>SUM(H7:S7)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U7"/>
+      <c s="32" r="U7"/>
     </row>
     <row r="8">
-      <c s="18" r="A8">
+      <c s="19" r="A8">
         <v>2.0</v>
       </c>
-      <c t="s" s="24" r="B8">
+      <c t="s" s="25" r="B8">
         <v>26</v>
       </c>
-      <c s="25" r="E8"/>
-      <c s="32" r="F8">
+      <c s="26" r="E8"/>
+      <c s="33" r="F8">
         <v>4.0</v>
       </c>
-      <c t="s" s="27" r="G8">
+      <c t="s" s="28" r="G8">
         <v>27</v>
       </c>
-      <c s="28" r="H8"/>
-      <c s="28" r="I8"/>
-      <c s="27" r="J8"/>
-      <c t="s" s="29" r="K8">
+      <c s="29" r="H8"/>
+      <c s="29" r="I8"/>
+      <c s="28" r="J8"/>
+      <c t="s" s="30" r="K8">
         <v>28</v>
       </c>
-      <c t="s" s="29" r="L8">
+      <c t="s" s="30" r="L8">
         <v>29</v>
       </c>
-      <c s="27" r="M8">
+      <c s="28" r="M8">
         <v>4.0</v>
       </c>
-      <c s="28" r="N8"/>
-      <c s="28" r="O8"/>
-      <c s="28" r="P8"/>
-      <c s="28" r="Q8"/>
-      <c s="28" r="R8"/>
-      <c s="28" r="S8"/>
-      <c t="str" s="33" r="T8">
+      <c s="29" r="N8"/>
+      <c s="29" r="O8"/>
+      <c s="29" r="P8"/>
+      <c s="29" r="Q8"/>
+      <c s="29" r="R8"/>
+      <c s="29" r="S8"/>
+      <c t="str" s="34" r="T8">
         <f>SUM(H8:S8)</f>
         <v>4</v>
       </c>
-      <c s="31" r="U8"/>
+      <c s="32" r="U8"/>
     </row>
     <row r="9">
-      <c s="18" r="A9">
+      <c s="19" r="A9">
         <v>3.0</v>
       </c>
-      <c t="s" s="24" r="B9">
+      <c t="s" s="25" r="B9">
         <v>30</v>
       </c>
-      <c s="25" r="E9"/>
-      <c s="32" r="F9">
+      <c s="26" r="E9"/>
+      <c s="33" r="F9">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G9">
+      <c t="s" s="28" r="G9">
         <v>31</v>
       </c>
-      <c s="28" r="H9"/>
-      <c s="28" r="I9"/>
-      <c s="28" r="J9"/>
-      <c t="s" s="29" r="K9">
+      <c s="29" r="H9"/>
+      <c s="29" r="I9"/>
+      <c s="29" r="J9"/>
+      <c t="s" s="30" r="K9">
         <v>32</v>
       </c>
-      <c t="s" s="29" r="L9">
+      <c t="s" s="30" r="L9">
         <v>33</v>
       </c>
-      <c s="27" r="M9">
+      <c s="28" r="M9">
         <v>16.0</v>
       </c>
-      <c s="28" r="N9"/>
-      <c s="28" r="O9"/>
-      <c s="28" r="P9"/>
-      <c s="28" r="Q9"/>
-      <c s="28" r="R9"/>
-      <c s="28" r="S9"/>
-      <c t="str" s="33" r="T9">
+      <c s="29" r="N9"/>
+      <c s="29" r="O9"/>
+      <c s="29" r="P9"/>
+      <c s="29" r="Q9"/>
+      <c s="29" r="R9"/>
+      <c s="29" r="S9"/>
+      <c t="str" s="34" r="T9">
         <f>SUM(H9:S9)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U9"/>
+      <c s="32" r="U9"/>
     </row>
     <row r="10">
-      <c s="18" r="A10">
+      <c s="19" r="A10">
         <v>4.0</v>
       </c>
-      <c t="s" s="24" r="B10">
+      <c t="s" s="25" r="B10">
         <v>34</v>
       </c>
-      <c s="25" r="E10"/>
-      <c s="32" r="F10">
+      <c s="26" r="E10"/>
+      <c s="33" r="F10">
         <v>4.0</v>
       </c>
-      <c t="s" s="27" r="G10">
+      <c t="s" s="28" r="G10">
         <v>35</v>
       </c>
-      <c s="28" r="H10"/>
-      <c s="28" r="I10"/>
-      <c s="28" r="J10"/>
-      <c t="s" s="29" r="K10">
+      <c s="29" r="H10"/>
+      <c s="29" r="I10"/>
+      <c s="29" r="J10"/>
+      <c t="s" s="30" r="K10">
         <v>36</v>
       </c>
-      <c t="s" s="29" r="L10">
+      <c t="s" s="30" r="L10">
         <v>37</v>
       </c>
-      <c s="27" r="M10">
+      <c s="28" r="M10">
         <v>4.0</v>
       </c>
-      <c s="28" r="N10"/>
-      <c s="28" r="O10"/>
-      <c s="28" r="P10"/>
-      <c s="28" r="Q10"/>
-      <c s="28" r="R10"/>
-      <c s="28" r="S10"/>
-      <c t="str" s="33" r="T10">
+      <c s="29" r="N10"/>
+      <c s="29" r="O10"/>
+      <c s="29" r="P10"/>
+      <c s="29" r="Q10"/>
+      <c s="29" r="R10"/>
+      <c s="29" r="S10"/>
+      <c t="str" s="34" r="T10">
         <f>SUM(H10:S10)</f>
         <v>4</v>
       </c>
-      <c s="31" r="U10"/>
+      <c s="32" r="U10"/>
     </row>
     <row r="11">
-      <c s="18" r="A11">
+      <c s="19" r="A11">
         <v>5.0</v>
       </c>
-      <c t="s" s="24" r="B11">
+      <c t="s" s="25" r="B11">
         <v>38</v>
       </c>
-      <c s="25" r="E11"/>
-      <c s="32" r="F11">
+      <c s="26" r="E11"/>
+      <c s="33" r="F11">
         <v>8.0</v>
       </c>
-      <c t="s" s="27" r="G11">
+      <c t="s" s="28" r="G11">
         <v>39</v>
       </c>
-      <c s="27" r="H11"/>
-      <c s="27" r="I11"/>
-      <c s="27" r="J11"/>
-      <c t="s" s="29" r="K11">
+      <c s="28" r="H11"/>
+      <c s="28" r="I11"/>
+      <c s="28" r="J11"/>
+      <c t="s" s="30" r="K11">
         <v>40</v>
       </c>
-      <c t="s" s="29" r="L11">
+      <c t="s" s="30" r="L11">
         <v>41</v>
       </c>
-      <c s="27" r="M11">
+      <c s="28" r="M11">
         <v>8.0</v>
       </c>
-      <c s="28" r="N11"/>
-      <c s="28" r="O11"/>
-      <c s="28" r="P11"/>
-      <c s="28" r="Q11"/>
-      <c s="28" r="R11"/>
-      <c s="28" r="S11"/>
-      <c t="str" s="33" r="T11">
+      <c s="29" r="N11"/>
+      <c s="29" r="O11"/>
+      <c s="29" r="P11"/>
+      <c s="29" r="Q11"/>
+      <c s="29" r="R11"/>
+      <c s="29" r="S11"/>
+      <c t="str" s="34" r="T11">
         <f>SUM(H11:S11)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U11"/>
+      <c s="32" r="U11"/>
     </row>
     <row r="12">
-      <c s="18" r="A12">
+      <c s="19" r="A12">
         <v>6.0</v>
       </c>
-      <c t="s" s="24" r="B12">
+      <c t="s" s="25" r="B12">
         <v>42</v>
       </c>
-      <c s="25" r="E12"/>
-      <c s="32" r="F12">
+      <c s="26" r="E12"/>
+      <c s="33" r="F12">
         <v>10.0</v>
       </c>
-      <c t="s" s="27" r="G12">
+      <c t="s" s="28" r="G12">
         <v>43</v>
       </c>
-      <c s="28" r="H12"/>
-      <c s="28" r="I12"/>
-      <c s="28" r="J12"/>
-      <c t="s" s="29" r="K12">
+      <c s="29" r="H12"/>
+      <c s="29" r="I12"/>
+      <c s="29" r="J12"/>
+      <c t="s" s="30" r="K12">
         <v>44</v>
       </c>
-      <c t="s" s="29" r="L12">
+      <c t="s" s="30" r="L12">
         <v>45</v>
       </c>
-      <c s="27" r="M12">
+      <c s="28" r="M12">
         <v>10.0</v>
       </c>
-      <c s="27" r="N12"/>
-      <c s="28" r="O12"/>
-      <c s="28" r="P12"/>
-      <c s="28" r="Q12"/>
-      <c s="28" r="R12"/>
-      <c s="28" r="S12"/>
-      <c t="str" s="33" r="T12">
+      <c s="28" r="N12"/>
+      <c s="29" r="O12"/>
+      <c s="29" r="P12"/>
+      <c s="29" r="Q12"/>
+      <c s="29" r="R12"/>
+      <c s="29" r="S12"/>
+      <c t="str" s="34" r="T12">
         <f>SUM(H12:S12)</f>
         <v>10</v>
       </c>
-      <c s="31" r="U12"/>
+      <c s="32" r="U12"/>
     </row>
     <row r="13">
-      <c s="18" r="A13">
+      <c s="19" r="A13">
         <v>7.0</v>
       </c>
-      <c t="s" s="24" r="B13">
+      <c t="s" s="25" r="B13">
         <v>46</v>
       </c>
-      <c s="25" r="E13"/>
-      <c s="32" r="F13">
+      <c s="26" r="E13"/>
+      <c s="33" r="F13">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G13">
+      <c t="s" s="28" r="G13">
         <v>47</v>
       </c>
-      <c s="28" r="H13"/>
-      <c s="28" r="I13"/>
-      <c s="28" r="J13"/>
-      <c t="s" s="29" r="K13">
+      <c s="29" r="H13"/>
+      <c s="29" r="I13"/>
+      <c s="29" r="J13"/>
+      <c t="s" s="30" r="K13">
         <v>48</v>
       </c>
-      <c t="s" s="29" r="L13">
+      <c t="s" s="30" r="L13">
         <v>49</v>
       </c>
-      <c s="27" r="M13">
+      <c s="28" r="M13">
         <v>8.0</v>
       </c>
-      <c s="27" r="N13">
+      <c s="28" r="N13">
         <v>8.0</v>
       </c>
-      <c s="27" r="O13"/>
-      <c s="27" r="P13"/>
-      <c s="28" r="Q13"/>
-      <c s="28" r="R13"/>
-      <c s="28" r="S13"/>
-      <c t="str" s="33" r="T13">
+      <c s="28" r="O13"/>
+      <c s="28" r="P13"/>
+      <c s="29" r="Q13"/>
+      <c s="29" r="R13"/>
+      <c s="29" r="S13"/>
+      <c t="str" s="34" r="T13">
         <f>SUM(H13:S13)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U13"/>
+      <c s="32" r="U13"/>
     </row>
     <row r="14">
-      <c s="18" r="A14">
+      <c s="19" r="A14">
         <v>8.0</v>
       </c>
-      <c t="s" s="24" r="B14">
+      <c t="s" s="25" r="B14">
         <v>50</v>
       </c>
-      <c s="25" r="E14"/>
-      <c s="32" r="F14">
+      <c s="26" r="E14"/>
+      <c s="33" r="F14">
         <v>10.0</v>
       </c>
-      <c t="s" s="27" r="G14">
+      <c t="s" s="28" r="G14">
         <v>51</v>
       </c>
-      <c s="28" r="H14"/>
-      <c s="28" r="I14"/>
-      <c s="28" r="J14"/>
-      <c t="s" s="29" r="K14">
+      <c s="29" r="H14"/>
+      <c s="29" r="I14"/>
+      <c s="29" r="J14"/>
+      <c t="s" s="30" r="K14">
         <v>52</v>
       </c>
-      <c t="s" s="29" r="L14">
+      <c t="s" s="30" r="L14">
         <v>53</v>
       </c>
-      <c s="27" r="M14">
+      <c s="28" r="M14">
         <v>10.0</v>
       </c>
-      <c s="27" r="N14"/>
-      <c s="27" r="O14"/>
-      <c s="27" r="P14"/>
-      <c s="28" r="Q14"/>
-      <c s="28" r="R14"/>
-      <c s="28" r="S14"/>
-      <c t="str" s="33" r="T14">
+      <c s="28" r="N14"/>
+      <c s="28" r="O14"/>
+      <c s="28" r="P14"/>
+      <c s="29" r="Q14"/>
+      <c s="29" r="R14"/>
+      <c s="29" r="S14"/>
+      <c t="str" s="34" r="T14">
         <f>SUM(H14:S14)</f>
         <v>10</v>
       </c>
-      <c s="31" r="U14"/>
+      <c s="32" r="U14"/>
     </row>
     <row r="15">
-      <c s="18" r="A15">
+      <c s="19" r="A15">
         <v>9.0</v>
       </c>
-      <c t="s" s="24" r="B15">
+      <c t="s" s="25" r="B15">
         <v>54</v>
       </c>
-      <c s="25" r="E15"/>
-      <c s="32" r="F15">
+      <c s="26" r="E15"/>
+      <c s="33" r="F15">
         <v>2.0</v>
       </c>
-      <c t="s" s="27" r="G15">
+      <c t="s" s="28" r="G15">
         <v>55</v>
       </c>
-      <c s="28" r="H15"/>
-      <c s="28" r="I15"/>
-      <c s="28" r="J15"/>
-      <c t="s" s="29" r="K15">
+      <c s="29" r="H15"/>
+      <c s="29" r="I15"/>
+      <c s="29" r="J15"/>
+      <c t="s" s="30" r="K15">
         <v>56</v>
       </c>
-      <c t="s" s="29" r="L15">
+      <c t="s" s="30" r="L15">
         <v>57</v>
       </c>
-      <c s="27" r="M15">
+      <c s="28" r="M15">
         <v>2.0</v>
       </c>
-      <c s="28" r="N15"/>
-      <c s="28" r="O15"/>
-      <c s="27" r="P15"/>
-      <c s="27" r="Q15"/>
-      <c s="28" r="R15"/>
-      <c s="28" r="S15"/>
-      <c t="str" s="33" r="T15">
+      <c s="29" r="N15"/>
+      <c s="29" r="O15"/>
+      <c s="28" r="P15"/>
+      <c s="28" r="Q15"/>
+      <c s="29" r="R15"/>
+      <c s="29" r="S15"/>
+      <c t="str" s="34" r="T15">
         <f>SUM(H15:S15)</f>
         <v>2</v>
       </c>
-      <c s="31" r="U15"/>
+      <c s="32" r="U15"/>
     </row>
     <row r="16">
-      <c s="18" r="A16">
+      <c s="19" r="A16">
         <v>10.0</v>
       </c>
-      <c t="s" s="24" r="B16">
+      <c t="s" s="25" r="B16">
         <v>58</v>
       </c>
-      <c s="25" r="E16"/>
-      <c s="32" r="F16">
+      <c s="26" r="E16"/>
+      <c s="33" r="F16">
         <v>2.0</v>
       </c>
-      <c t="s" s="27" r="G16">
+      <c t="s" s="28" r="G16">
         <v>59</v>
       </c>
-      <c s="28" r="H16"/>
-      <c s="28" r="I16"/>
-      <c s="28" r="J16"/>
-      <c t="s" s="29" r="K16">
+      <c s="29" r="H16"/>
+      <c s="29" r="I16"/>
+      <c s="29" r="J16"/>
+      <c t="s" s="30" r="K16">
         <v>60</v>
       </c>
-      <c t="s" s="29" r="L16">
+      <c t="s" s="30" r="L16">
         <v>61</v>
       </c>
-      <c s="27" r="M16">
+      <c s="28" r="M16">
         <v>2.0</v>
       </c>
-      <c s="28" r="N16"/>
-      <c s="28" r="O16"/>
-      <c s="28" r="P16"/>
-      <c s="28" r="Q16"/>
-      <c s="28" r="R16"/>
-      <c s="28" r="S16"/>
-      <c t="str" s="33" r="T16">
+      <c s="29" r="N16"/>
+      <c s="29" r="O16"/>
+      <c s="29" r="P16"/>
+      <c s="29" r="Q16"/>
+      <c s="29" r="R16"/>
+      <c s="29" r="S16"/>
+      <c t="str" s="34" r="T16">
         <f>SUM(H16:S16)</f>
         <v>2</v>
       </c>
-      <c s="31" r="U16"/>
+      <c s="32" r="U16"/>
     </row>
     <row r="17">
-      <c s="18" r="A17">
+      <c s="19" r="A17">
         <v>11.0</v>
       </c>
-      <c t="s" s="24" r="B17">
+      <c t="s" s="25" r="B17">
         <v>62</v>
       </c>
-      <c s="25" r="E17"/>
-      <c s="32" r="F17">
+      <c s="26" r="E17"/>
+      <c s="33" r="F17">
         <v>2.0</v>
       </c>
-      <c t="s" s="27" r="G17">
+      <c t="s" s="28" r="G17">
         <v>63</v>
       </c>
-      <c s="28" r="H17"/>
-      <c s="28" r="I17"/>
-      <c s="28" r="J17"/>
-      <c t="s" s="29" r="K17">
+      <c s="29" r="H17"/>
+      <c s="29" r="I17"/>
+      <c s="29" r="J17"/>
+      <c t="s" s="30" r="K17">
         <v>64</v>
       </c>
-      <c t="s" s="29" r="L17">
+      <c t="s" s="30" r="L17">
         <v>65</v>
       </c>
-      <c s="27" r="M17">
+      <c s="28" r="M17">
         <v>2.0</v>
       </c>
-      <c s="28" r="N17"/>
-      <c s="28" r="O17"/>
-      <c s="28" r="P17"/>
-      <c s="28" r="Q17"/>
-      <c s="28" r="R17"/>
-      <c s="28" r="S17"/>
-      <c t="str" s="33" r="T17">
+      <c s="29" r="N17"/>
+      <c s="29" r="O17"/>
+      <c s="29" r="P17"/>
+      <c s="29" r="Q17"/>
+      <c s="29" r="R17"/>
+      <c s="29" r="S17"/>
+      <c t="str" s="34" r="T17">
         <f>SUM(H17:S17)</f>
         <v>2</v>
       </c>
-      <c s="31" r="U17"/>
+      <c s="32" r="U17"/>
     </row>
     <row r="18">
-      <c s="18" r="A18">
+      <c s="19" r="A18">
         <v>12.0</v>
       </c>
-      <c t="s" s="24" r="B18">
+      <c t="s" s="25" r="B18">
         <v>66</v>
       </c>
-      <c s="25" r="E18">
+      <c s="26" r="E18">
         <v>6.0</v>
       </c>
-      <c s="32" r="F18">
+      <c s="33" r="F18">
         <v>10.0</v>
       </c>
-      <c t="s" s="27" r="G18">
+      <c t="s" s="28" r="G18">
         <v>67</v>
       </c>
-      <c s="28" r="H18"/>
-      <c s="28" r="I18"/>
-      <c s="28" r="J18"/>
-      <c t="s" s="29" r="K18">
+      <c s="29" r="H18"/>
+      <c s="29" r="I18"/>
+      <c s="29" r="J18"/>
+      <c t="s" s="30" r="K18">
         <v>68</v>
       </c>
-      <c t="s" s="29" r="L18">
+      <c t="s" s="30" r="L18">
         <v>69</v>
       </c>
-      <c s="27" r="M18">
+      <c s="28" r="M18">
         <v>10.0</v>
       </c>
-      <c s="28" r="N18"/>
-      <c s="28" r="O18"/>
-      <c s="28" r="P18"/>
-      <c s="28" r="Q18"/>
-      <c s="28" r="R18"/>
-      <c s="28" r="S18"/>
-      <c t="str" s="33" r="T18">
+      <c s="29" r="N18"/>
+      <c s="29" r="O18"/>
+      <c s="29" r="P18"/>
+      <c s="29" r="Q18"/>
+      <c s="29" r="R18"/>
+      <c s="29" r="S18"/>
+      <c t="str" s="34" r="T18">
         <f>SUM(H18:S18)</f>
         <v>10</v>
       </c>
-      <c s="31" r="U18"/>
+      <c s="32" r="U18"/>
     </row>
     <row r="19">
-      <c s="18" r="A19">
+      <c s="19" r="A19">
         <v>13.0</v>
       </c>
-      <c t="s" s="24" r="B19">
+      <c t="s" s="25" r="B19">
         <v>70</v>
       </c>
-      <c s="25" r="E19">
+      <c s="26" r="E19">
         <v>6.0</v>
       </c>
-      <c s="32" r="F19">
+      <c s="33" r="F19">
         <v>4.0</v>
       </c>
-      <c t="s" s="27" r="G19">
+      <c t="s" s="28" r="G19">
         <v>71</v>
       </c>
-      <c s="28" r="H19"/>
-      <c s="28" r="I19"/>
-      <c s="28" r="J19"/>
-      <c t="s" s="29" r="K19">
+      <c s="29" r="H19"/>
+      <c s="29" r="I19"/>
+      <c s="29" r="J19"/>
+      <c t="s" s="30" r="K19">
         <v>72</v>
       </c>
-      <c t="s" s="29" r="L19">
+      <c t="s" s="30" r="L19">
         <v>73</v>
       </c>
-      <c s="27" r="M19">
+      <c s="28" r="M19">
         <v>4.0</v>
       </c>
-      <c s="28" r="N19"/>
-      <c s="28" r="O19"/>
-      <c s="28" r="P19"/>
-      <c s="28" r="Q19"/>
-      <c s="28" r="R19"/>
-      <c s="28" r="S19"/>
-      <c t="str" s="33" r="T19">
+      <c s="29" r="N19"/>
+      <c s="29" r="O19"/>
+      <c s="29" r="P19"/>
+      <c s="29" r="Q19"/>
+      <c s="29" r="R19"/>
+      <c s="29" r="S19"/>
+      <c t="str" s="34" r="T19">
         <f>SUM(H19:S19)</f>
         <v>4</v>
       </c>
-      <c s="31" r="U19"/>
+      <c s="32" r="U19"/>
     </row>
     <row r="20">
-      <c s="18" r="A20">
+      <c s="19" r="A20">
         <v>14.0</v>
       </c>
-      <c t="s" s="24" r="B20">
+      <c t="s" s="25" r="B20">
         <v>74</v>
       </c>
-      <c s="25" r="E20">
+      <c s="26" r="E20">
         <v>7.0</v>
       </c>
-      <c s="32" r="F20">
+      <c s="33" r="F20">
         <v>20.0</v>
       </c>
-      <c t="s" s="27" r="G20">
+      <c t="s" s="28" r="G20">
         <v>75</v>
       </c>
-      <c s="28" r="H20"/>
-      <c s="28" r="I20"/>
-      <c s="28" r="J20"/>
-      <c t="s" s="29" r="K20">
+      <c s="29" r="H20"/>
+      <c s="29" r="I20"/>
+      <c s="29" r="J20"/>
+      <c t="s" s="30" r="K20">
         <v>76</v>
       </c>
-      <c t="s" s="29" r="L20">
+      <c t="s" s="30" r="L20">
         <v>77</v>
       </c>
-      <c s="28" r="M20"/>
-      <c s="27" r="N20"/>
-      <c s="28" r="O20"/>
-      <c s="28" r="P20"/>
-      <c s="27" r="Q20"/>
-      <c s="27" r="R20">
+      <c s="29" r="M20"/>
+      <c s="28" r="N20"/>
+      <c s="29" r="O20"/>
+      <c s="29" r="P20"/>
+      <c s="28" r="Q20"/>
+      <c s="28" r="R20">
         <v>20.0</v>
       </c>
-      <c s="28" r="S20"/>
-      <c t="str" s="33" r="T20">
+      <c s="29" r="S20"/>
+      <c t="str" s="34" r="T20">
         <f>SUM(H20:S20)</f>
         <v>20</v>
       </c>
-      <c s="31" r="U20"/>
+      <c s="32" r="U20"/>
     </row>
     <row r="21">
-      <c s="18" r="A21">
+      <c s="19" r="A21">
         <v>15.0</v>
       </c>
-      <c t="s" s="24" r="B21">
+      <c t="s" s="25" r="B21">
         <v>78</v>
       </c>
-      <c s="25" r="E21">
+      <c s="26" r="E21">
         <v>8.0</v>
       </c>
-      <c s="26" r="F21">
+      <c s="27" r="F21">
         <v>8.0</v>
       </c>
-      <c t="s" s="34" r="G21">
+      <c t="s" s="35" r="G21">
         <v>79</v>
       </c>
-      <c s="35" r="H21"/>
-      <c s="35" r="I21"/>
-      <c s="35" r="J21"/>
-      <c t="s" s="29" r="K21">
+      <c s="36" r="H21"/>
+      <c s="36" r="I21"/>
+      <c s="36" r="J21"/>
+      <c t="s" s="30" r="K21">
         <v>80</v>
       </c>
-      <c t="s" s="29" r="L21">
+      <c t="s" s="30" r="L21">
         <v>81</v>
       </c>
-      <c s="35" r="M21"/>
-      <c s="35" r="N21">
+      <c s="36" r="M21"/>
+      <c s="36" r="N21">
         <v>8.0</v>
       </c>
-      <c s="35" r="O21"/>
-      <c s="35" r="P21"/>
-      <c s="35" r="Q21"/>
-      <c s="36" r="R21"/>
-      <c s="36" r="S21"/>
-      <c t="str" s="33" r="T21">
+      <c s="36" r="O21"/>
+      <c s="36" r="P21"/>
+      <c s="36" r="Q21"/>
+      <c s="37" r="R21"/>
+      <c s="37" r="S21"/>
+      <c t="str" s="34" r="T21">
         <f>SUM(H21:S21)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U21"/>
+      <c s="32" r="U21"/>
     </row>
     <row r="22">
-      <c s="18" r="A22">
+      <c s="19" r="A22">
         <v>16.0</v>
       </c>
-      <c t="s" s="24" r="B22">
+      <c t="s" s="25" r="B22">
         <v>82</v>
       </c>
-      <c s="25" r="E22">
+      <c s="26" r="E22">
         <v>10.0</v>
       </c>
-      <c s="32" r="F22">
+      <c s="33" r="F22">
         <v>8.0</v>
       </c>
-      <c t="s" s="27" r="G22">
+      <c t="s" s="28" r="G22">
         <v>83</v>
       </c>
-      <c s="28" r="H22"/>
-      <c s="28" r="I22"/>
-      <c s="28" r="J22"/>
-      <c t="s" s="29" r="K22">
+      <c s="29" r="H22"/>
+      <c s="29" r="I22"/>
+      <c s="29" r="J22"/>
+      <c t="s" s="30" r="K22">
         <v>84</v>
       </c>
-      <c t="s" s="29" r="L22">
+      <c t="s" s="30" r="L22">
         <v>85</v>
       </c>
-      <c s="28" r="M22"/>
-      <c s="27" r="N22">
+      <c s="29" r="M22"/>
+      <c s="28" r="N22">
         <v>8.0</v>
       </c>
-      <c s="28" r="O22"/>
-      <c s="28" r="P22"/>
-      <c s="28" r="Q22"/>
-      <c s="28" r="R22"/>
-      <c s="28" r="S22"/>
-      <c t="str" s="33" r="T22">
+      <c s="29" r="O22"/>
+      <c s="29" r="P22"/>
+      <c s="29" r="Q22"/>
+      <c s="29" r="R22"/>
+      <c s="29" r="S22"/>
+      <c t="str" s="34" r="T22">
         <f>SUM(H22:S22)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U22"/>
+      <c s="32" r="U22"/>
     </row>
     <row r="23">
-      <c s="18" r="A23">
+      <c s="19" r="A23">
         <v>17.0</v>
       </c>
-      <c t="s" s="24" r="B23">
+      <c t="s" s="25" r="B23">
         <v>86</v>
       </c>
-      <c s="25" r="E23">
+      <c s="26" r="E23">
         <v>11.0</v>
       </c>
-      <c s="32" r="F23">
+      <c s="33" r="F23">
         <v>20.0</v>
       </c>
-      <c t="s" s="27" r="G23">
+      <c t="s" s="28" r="G23">
         <v>87</v>
       </c>
-      <c s="28" r="H23"/>
-      <c s="28" r="I23"/>
-      <c s="28" r="J23"/>
-      <c t="s" s="29" r="K23">
+      <c s="29" r="H23"/>
+      <c s="29" r="I23"/>
+      <c s="29" r="J23"/>
+      <c t="s" s="30" r="K23">
         <v>88</v>
       </c>
-      <c t="s" s="29" r="L23">
+      <c t="s" s="30" r="L23">
         <v>89</v>
       </c>
-      <c s="28" r="M23"/>
-      <c s="27" r="N23">
+      <c s="29" r="M23"/>
+      <c s="28" r="N23">
         <v>20.0</v>
       </c>
-      <c s="28" r="O23"/>
-      <c s="28" r="P23"/>
-      <c s="28" r="Q23"/>
-      <c s="28" r="R23"/>
-      <c s="28" r="S23"/>
-      <c t="str" s="33" r="T23">
+      <c s="29" r="O23"/>
+      <c s="29" r="P23"/>
+      <c s="29" r="Q23"/>
+      <c s="29" r="R23"/>
+      <c s="29" r="S23"/>
+      <c t="str" s="34" r="T23">
         <f>SUM(H23:S23)</f>
         <v>20</v>
       </c>
-      <c s="31" r="U23"/>
+      <c s="32" r="U23"/>
     </row>
     <row r="24">
-      <c s="18" r="A24">
+      <c s="19" r="A24">
         <v>18.0</v>
       </c>
-      <c t="s" s="24" r="B24">
+      <c t="s" s="25" r="B24">
         <v>90</v>
       </c>
-      <c t="s" s="25" r="E24">
+      <c t="s" s="26" r="E24">
         <v>91</v>
       </c>
-      <c s="32" r="F24">
+      <c s="33" r="F24">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G24">
+      <c t="s" s="28" r="G24">
         <v>92</v>
       </c>
-      <c s="28" r="H24"/>
-      <c s="28" r="I24"/>
-      <c s="28" r="J24"/>
-      <c t="s" s="29" r="K24">
+      <c s="29" r="H24"/>
+      <c s="29" r="I24"/>
+      <c s="29" r="J24"/>
+      <c t="s" s="30" r="K24">
         <v>93</v>
       </c>
-      <c t="s" s="29" r="L24">
+      <c t="s" s="30" r="L24">
         <v>94</v>
       </c>
-      <c s="28" r="M24"/>
-      <c s="27" r="N24">
+      <c s="29" r="M24"/>
+      <c s="28" r="N24">
         <v>16.0</v>
       </c>
-      <c s="28" r="O24"/>
-      <c s="28" r="P24"/>
-      <c s="28" r="Q24"/>
-      <c s="28" r="R24"/>
-      <c s="28" r="S24"/>
-      <c t="str" s="33" r="T24">
+      <c s="29" r="O24"/>
+      <c s="29" r="P24"/>
+      <c s="29" r="Q24"/>
+      <c s="29" r="R24"/>
+      <c s="29" r="S24"/>
+      <c t="str" s="34" r="T24">
         <f>SUM(H24:S24)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U24"/>
+      <c s="32" r="U24"/>
     </row>
     <row r="25">
-      <c s="18" r="A25">
+      <c s="19" r="A25">
         <v>19.0</v>
       </c>
-      <c t="s" s="24" r="B25">
+      <c t="s" s="25" r="B25">
         <v>95</v>
       </c>
-      <c t="s" s="25" r="E25">
+      <c t="s" s="26" r="E25">
         <v>96</v>
       </c>
-      <c s="32" r="F25">
+      <c s="33" r="F25">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G25">
+      <c t="s" s="28" r="G25">
         <v>97</v>
       </c>
-      <c s="37" r="H25"/>
-      <c s="37" r="I25"/>
-      <c s="38" r="J25"/>
-      <c t="s" s="29" r="K25">
+      <c s="38" r="H25"/>
+      <c s="38" r="I25"/>
+      <c s="39" r="J25"/>
+      <c t="s" s="30" r="K25">
         <v>98</v>
       </c>
-      <c t="s" s="29" r="L25">
+      <c t="s" s="30" r="L25">
         <v>99</v>
       </c>
-      <c s="38" r="M25"/>
-      <c s="38" r="N25">
+      <c s="39" r="M25"/>
+      <c s="39" r="N25">
         <v>16.0</v>
       </c>
-      <c s="37" r="O25"/>
-      <c s="37" r="P25"/>
-      <c s="37" r="Q25"/>
-      <c s="37" r="R25"/>
-      <c s="37" r="S25"/>
-      <c t="str" s="33" r="T25">
+      <c s="38" r="O25"/>
+      <c s="38" r="P25"/>
+      <c s="38" r="Q25"/>
+      <c s="38" r="R25"/>
+      <c s="38" r="S25"/>
+      <c t="str" s="34" r="T25">
         <f>SUM(H25:S25)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U25"/>
+      <c s="32" r="U25"/>
     </row>
     <row r="26">
-      <c s="18" r="A26">
+      <c s="19" r="A26">
         <v>24.0</v>
       </c>
-      <c t="s" s="24" r="B26">
+      <c t="s" s="25" r="B26">
         <v>100</v>
       </c>
-      <c s="25" r="E26">
+      <c s="26" r="E26">
         <v>13.0</v>
       </c>
-      <c s="39" r="F26">
+      <c s="40" r="F26">
         <v>40.0</v>
       </c>
-      <c t="s" s="27" r="G26">
+      <c t="s" s="28" r="G26">
         <v>101</v>
       </c>
-      <c s="28" r="H26"/>
-      <c s="28" r="I26"/>
-      <c s="28" r="J26"/>
-      <c t="s" s="29" r="K26">
+      <c s="29" r="H26"/>
+      <c s="29" r="I26"/>
+      <c s="29" r="J26"/>
+      <c t="s" s="30" r="K26">
         <v>102</v>
       </c>
-      <c t="s" s="29" r="L26">
+      <c t="s" s="30" r="L26">
         <v>103</v>
       </c>
-      <c s="28" r="M26"/>
-      <c s="28" r="N26"/>
-      <c s="28" r="O26"/>
-      <c s="27" r="P26"/>
-      <c s="27" r="Q26">
+      <c s="29" r="M26"/>
+      <c s="29" r="N26"/>
+      <c s="29" r="O26"/>
+      <c s="28" r="P26"/>
+      <c s="28" r="Q26">
         <v>16.0</v>
       </c>
-      <c s="27" r="R26">
+      <c s="28" r="R26">
         <v>24.0</v>
       </c>
-      <c s="28" r="S26"/>
-      <c t="str" s="33" r="T26">
+      <c s="29" r="S26"/>
+      <c t="str" s="34" r="T26">
         <f>SUM(H26:S26)</f>
         <v>40</v>
       </c>
-      <c s="31" r="U26"/>
+      <c s="32" r="U26"/>
     </row>
     <row r="27">
-      <c s="18" r="A27">
+      <c s="19" r="A27">
         <v>25.0</v>
       </c>
-      <c t="s" s="24" r="B27">
+      <c t="s" s="25" r="B27">
         <v>104</v>
       </c>
-      <c t="s" s="25" r="E27">
+      <c t="s" s="26" r="E27">
         <v>105</v>
       </c>
-      <c s="40" r="F27">
+      <c s="41" r="F27">
         <v>16.0</v>
       </c>
-      <c t="s" s="27" r="G27">
+      <c t="s" s="28" r="G27">
         <v>106</v>
       </c>
-      <c s="28" r="H27"/>
-      <c s="28" r="I27"/>
-      <c s="28" r="J27"/>
-      <c t="s" s="29" r="K27">
+      <c s="29" r="H27"/>
+      <c s="29" r="I27"/>
+      <c s="29" r="J27"/>
+      <c t="s" s="30" r="K27">
         <v>107</v>
       </c>
-      <c t="s" s="29" r="L27">
+      <c t="s" s="30" r="L27">
         <v>108</v>
       </c>
-      <c s="27" r="M27"/>
-      <c s="28" r="N27"/>
-      <c s="27" r="O27">
+      <c s="28" r="M27"/>
+      <c s="29" r="N27"/>
+      <c s="28" r="O27">
         <v>16.0</v>
       </c>
-      <c s="27" r="P27"/>
-      <c s="28" r="Q27"/>
-      <c s="28" r="R27"/>
-      <c s="28" r="S27"/>
-      <c t="str" s="33" r="T27">
+      <c s="28" r="P27"/>
+      <c s="29" r="Q27"/>
+      <c s="29" r="R27"/>
+      <c s="29" r="S27"/>
+      <c t="str" s="34" r="T27">
         <f>SUM(H27:S27)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U27"/>
+      <c s="32" r="U27"/>
     </row>
     <row r="28">
-      <c s="18" r="A28">
+      <c s="19" r="A28">
         <v>26.0</v>
       </c>
-      <c t="s" s="24" r="B28">
+      <c t="s" s="25" r="B28">
         <v>109</v>
       </c>
-      <c t="s" s="25" r="E28">
+      <c t="s" s="26" r="E28">
         <v>110</v>
       </c>
-      <c s="32" r="F28">
+      <c s="33" r="F28">
         <v>8.0</v>
       </c>
-      <c t="s" s="34" r="G28">
+      <c t="s" s="35" r="G28">
         <v>111</v>
       </c>
-      <c s="28" r="H28"/>
-      <c s="28" r="I28"/>
-      <c s="28" r="J28"/>
-      <c t="s" s="29" r="K28">
+      <c s="29" r="H28"/>
+      <c s="29" r="I28"/>
+      <c s="29" r="J28"/>
+      <c t="s" s="30" r="K28">
         <v>112</v>
       </c>
-      <c t="s" s="29" r="L28">
+      <c t="s" s="30" r="L28">
         <v>113</v>
       </c>
-      <c s="28" r="M28"/>
-      <c s="28" r="N28"/>
-      <c s="27" r="O28">
+      <c s="29" r="M28"/>
+      <c s="29" r="N28"/>
+      <c s="28" r="O28">
         <v>8.0</v>
       </c>
-      <c s="28" r="P28"/>
-      <c s="28" r="Q28"/>
-      <c s="28" r="R28"/>
-      <c s="28" r="S28"/>
-      <c t="str" s="33" r="T28">
+      <c s="29" r="P28"/>
+      <c s="29" r="Q28"/>
+      <c s="29" r="R28"/>
+      <c s="29" r="S28"/>
+      <c t="str" s="34" r="T28">
         <f>SUM(H28:S28)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U28"/>
+      <c s="32" r="U28"/>
     </row>
     <row r="29">
-      <c s="18" r="A29">
+      <c s="19" r="A29">
         <v>27.0</v>
       </c>
-      <c t="s" s="24" r="B29">
+      <c t="s" s="25" r="B29">
         <v>114</v>
       </c>
-      <c t="s" s="25" r="E29">
+      <c t="s" s="26" r="E29">
         <v>115</v>
       </c>
-      <c s="39" r="F29">
+      <c s="40" r="F29">
         <v>12.0</v>
       </c>
-      <c t="s" s="41" r="G29">
+      <c t="s" s="42" r="G29">
         <v>116</v>
       </c>
-      <c s="28" r="H29"/>
-      <c s="28" r="I29"/>
-      <c s="28" r="J29"/>
-      <c t="s" s="29" r="K29">
+      <c s="29" r="H29"/>
+      <c s="29" r="I29"/>
+      <c s="29" r="J29"/>
+      <c t="s" s="30" r="K29">
         <v>117</v>
       </c>
-      <c t="s" s="29" r="L29">
+      <c t="s" s="30" r="L29">
         <v>118</v>
       </c>
-      <c s="28" r="M29"/>
-      <c s="28" r="N29"/>
-      <c s="27" r="O29">
+      <c s="29" r="M29"/>
+      <c s="29" r="N29"/>
+      <c s="28" r="O29">
         <v>12.0</v>
       </c>
-      <c s="28" r="P29"/>
-      <c s="28" r="Q29"/>
-      <c s="28" r="R29"/>
-      <c s="28" r="S29"/>
-      <c t="str" s="33" r="T29">
+      <c s="29" r="P29"/>
+      <c s="29" r="Q29"/>
+      <c s="29" r="R29"/>
+      <c s="29" r="S29"/>
+      <c t="str" s="34" r="T29">
         <f>SUM(H29:S29)</f>
         <v>12</v>
       </c>
-      <c s="31" r="U29"/>
+      <c s="32" r="U29"/>
     </row>
     <row r="30">
-      <c s="18" r="A30">
+      <c s="19" r="A30">
         <v>28.0</v>
       </c>
-      <c t="s" s="24" r="B30">
+      <c t="s" s="25" r="B30">
         <v>119</v>
       </c>
-      <c s="25" r="E30">
+      <c s="26" r="E30">
         <v>25.0</v>
       </c>
-      <c s="39" r="F30">
+      <c s="40" r="F30">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G30">
+      <c t="s" s="42" r="G30">
         <v>120</v>
       </c>
-      <c s="28" r="H30"/>
-      <c s="28" r="I30"/>
-      <c s="28" r="J30"/>
-      <c t="s" s="29" r="K30">
+      <c s="29" r="H30"/>
+      <c s="29" r="I30"/>
+      <c s="29" r="J30"/>
+      <c t="s" s="30" r="K30">
         <v>121</v>
       </c>
-      <c t="s" s="29" r="L30">
+      <c t="s" s="30" r="L30">
         <v>122</v>
       </c>
-      <c s="28" r="M30"/>
-      <c s="28" r="N30"/>
-      <c s="27" r="O30">
+      <c s="29" r="M30"/>
+      <c s="29" r="N30"/>
+      <c s="28" r="O30">
         <v>8.0</v>
       </c>
-      <c s="28" r="P30"/>
-      <c s="28" r="Q30"/>
-      <c s="28" r="R30"/>
-      <c s="28" r="S30"/>
-      <c t="str" s="33" r="T30">
+      <c s="29" r="P30"/>
+      <c s="29" r="Q30"/>
+      <c s="29" r="R30"/>
+      <c s="29" r="S30"/>
+      <c t="str" s="34" r="T30">
         <f>SUM(H30:S30)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U30"/>
+      <c s="32" r="U30"/>
     </row>
     <row r="31">
-      <c s="18" r="A31">
+      <c s="19" r="A31">
         <v>29.0</v>
       </c>
-      <c t="s" s="24" r="B31">
+      <c t="s" s="25" r="B31">
         <v>123</v>
       </c>
-      <c s="25" r="E31">
+      <c s="26" r="E31">
         <v>37.0</v>
       </c>
-      <c s="39" r="F31">
+      <c s="40" r="F31">
         <v>20.0</v>
       </c>
-      <c t="s" s="41" r="G31">
+      <c t="s" s="42" r="G31">
         <v>124</v>
       </c>
-      <c s="28" r="H31"/>
-      <c s="28" r="I31"/>
-      <c s="28" r="J31"/>
-      <c t="s" s="29" r="K31">
+      <c s="29" r="H31"/>
+      <c s="29" r="I31"/>
+      <c s="29" r="J31"/>
+      <c t="s" s="30" r="K31">
         <v>125</v>
       </c>
-      <c t="s" s="29" r="L31">
+      <c t="s" s="30" r="L31">
         <v>126</v>
       </c>
-      <c s="28" r="M31"/>
-      <c s="27" r="N31">
+      <c s="29" r="M31"/>
+      <c s="28" r="N31">
         <v>4.0</v>
       </c>
-      <c s="27" r="O31">
+      <c s="28" r="O31">
         <v>4.0</v>
       </c>
-      <c s="27" r="P31">
+      <c s="28" r="P31">
         <v>12.0</v>
       </c>
-      <c s="28" r="Q31"/>
-      <c s="27" r="R31"/>
-      <c s="27" r="S31"/>
-      <c t="str" s="33" r="T31">
+      <c s="29" r="Q31"/>
+      <c s="28" r="R31"/>
+      <c s="28" r="S31"/>
+      <c t="str" s="34" r="T31">
         <f>SUM(H31:S31)</f>
         <v>20</v>
       </c>
-      <c s="31" r="U31"/>
+      <c s="32" r="U31"/>
     </row>
     <row r="32">
-      <c s="18" r="A32">
+      <c s="19" r="A32">
         <v>30.0</v>
       </c>
-      <c t="s" s="24" r="B32">
+      <c t="s" s="25" r="B32">
         <v>127</v>
       </c>
-      <c t="s" s="25" r="E32">
+      <c t="s" s="26" r="E32">
         <v>128</v>
       </c>
-      <c s="39" r="F32">
+      <c s="40" r="F32">
         <v>16.0</v>
       </c>
-      <c t="s" s="41" r="G32">
+      <c t="s" s="42" r="G32">
         <v>129</v>
       </c>
-      <c s="28" r="H32"/>
-      <c s="28" r="I32"/>
-      <c s="28" r="J32"/>
-      <c t="s" s="29" r="K32">
+      <c s="29" r="H32"/>
+      <c s="29" r="I32"/>
+      <c s="29" r="J32"/>
+      <c t="s" s="30" r="K32">
         <v>130</v>
       </c>
-      <c t="s" s="29" r="L32">
+      <c t="s" s="30" r="L32">
         <v>131</v>
       </c>
-      <c s="28" r="M32"/>
-      <c s="28" r="N32"/>
-      <c s="27" r="O32">
+      <c s="29" r="M32"/>
+      <c s="29" r="N32"/>
+      <c s="28" r="O32">
         <v>16.0</v>
       </c>
-      <c s="28" r="P32"/>
-      <c s="28" r="Q32"/>
-      <c s="28" r="R32"/>
-      <c s="28" r="S32"/>
-      <c t="str" s="33" r="T32">
+      <c s="29" r="P32"/>
+      <c s="29" r="Q32"/>
+      <c s="29" r="R32"/>
+      <c s="29" r="S32"/>
+      <c t="str" s="34" r="T32">
         <f>SUM(H32:S32)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U32"/>
+      <c s="32" r="U32"/>
     </row>
     <row r="33">
-      <c s="18" r="A33">
+      <c s="19" r="A33">
         <v>31.0</v>
       </c>
-      <c t="s" s="24" r="B33">
+      <c t="s" s="25" r="B33">
         <v>132</v>
       </c>
-      <c s="25" r="E33">
+      <c s="26" r="E33">
         <v>26.0</v>
       </c>
-      <c s="39" r="F33">
+      <c s="40" r="F33">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G33">
+      <c t="s" s="42" r="G33">
         <v>133</v>
       </c>
-      <c s="28" r="H33"/>
-      <c s="28" r="I33"/>
-      <c s="28" r="J33"/>
-      <c t="s" s="29" r="K33">
+      <c s="29" r="H33"/>
+      <c s="29" r="I33"/>
+      <c s="29" r="J33"/>
+      <c t="s" s="30" r="K33">
         <v>134</v>
       </c>
-      <c t="s" s="29" r="L33">
+      <c t="s" s="30" r="L33">
         <v>135</v>
       </c>
-      <c s="28" r="M33"/>
-      <c s="27" r="N33">
+      <c s="29" r="M33"/>
+      <c s="28" r="N33">
         <v>8.0</v>
       </c>
-      <c s="27" r="O33"/>
-      <c s="28" r="P33"/>
-      <c s="28" r="Q33"/>
-      <c s="28" r="R33"/>
-      <c s="28" r="S33"/>
-      <c t="str" s="33" r="T33">
+      <c s="28" r="O33"/>
+      <c s="29" r="P33"/>
+      <c s="29" r="Q33"/>
+      <c s="29" r="R33"/>
+      <c s="29" r="S33"/>
+      <c t="str" s="34" r="T33">
         <f>SUM(H33:S33)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U33"/>
+      <c s="32" r="U33"/>
     </row>
     <row r="34">
-      <c s="18" r="A34">
+      <c s="19" r="A34">
         <v>32.0</v>
       </c>
-      <c t="s" s="24" r="B34">
+      <c t="s" s="25" r="B34">
         <v>136</v>
       </c>
-      <c s="25" r="E34">
+      <c s="26" r="E34">
         <v>26.0</v>
       </c>
-      <c s="39" r="F34">
+      <c s="40" r="F34">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G34">
+      <c t="s" s="42" r="G34">
         <v>137</v>
       </c>
-      <c s="28" r="H34"/>
-      <c s="28" r="I34"/>
-      <c s="28" r="J34"/>
-      <c t="s" s="29" r="K34">
+      <c s="29" r="H34"/>
+      <c s="29" r="I34"/>
+      <c s="29" r="J34"/>
+      <c t="s" s="30" r="K34">
         <v>138</v>
       </c>
-      <c t="s" s="29" r="L34">
+      <c t="s" s="30" r="L34">
         <v>139</v>
       </c>
-      <c s="28" r="M34"/>
-      <c s="27" r="N34">
+      <c s="29" r="M34"/>
+      <c s="28" r="N34">
         <v>8.0</v>
       </c>
-      <c s="27" r="O34"/>
-      <c s="28" r="P34"/>
-      <c s="28" r="Q34"/>
-      <c s="28" r="R34"/>
-      <c s="28" r="S34"/>
-      <c t="str" s="33" r="T34">
+      <c s="28" r="O34"/>
+      <c s="29" r="P34"/>
+      <c s="29" r="Q34"/>
+      <c s="29" r="R34"/>
+      <c s="29" r="S34"/>
+      <c t="str" s="34" r="T34">
         <f>SUM(H34:S34)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U34"/>
+      <c s="32" r="U34"/>
     </row>
     <row r="35">
-      <c s="18" r="A35">
+      <c s="19" r="A35">
         <v>33.0</v>
       </c>
-      <c t="s" s="24" r="B35">
+      <c t="s" s="25" r="B35">
         <v>140</v>
       </c>
-      <c t="s" s="25" r="E35">
+      <c t="s" s="26" r="E35">
         <v>141</v>
       </c>
-      <c s="42" r="F35">
+      <c s="43" r="F35">
         <v>8.0</v>
       </c>
-      <c t="s" s="43" r="G35">
+      <c t="s" s="44" r="G35">
         <v>142</v>
       </c>
-      <c s="36" r="H35"/>
-      <c s="36" r="I35"/>
-      <c s="36" r="J35"/>
-      <c t="s" s="29" r="K35">
+      <c s="37" r="H35"/>
+      <c s="37" r="I35"/>
+      <c s="37" r="J35"/>
+      <c t="s" s="30" r="K35">
         <v>143</v>
       </c>
-      <c t="s" s="29" r="L35">
+      <c t="s" s="30" r="L35">
         <v>144</v>
       </c>
-      <c s="36" r="M35"/>
-      <c s="36" r="N35"/>
-      <c s="35" r="O35">
+      <c s="37" r="M35"/>
+      <c s="37" r="N35"/>
+      <c s="36" r="O35">
         <v>8.0</v>
       </c>
-      <c s="36" r="P35"/>
-      <c s="36" r="Q35"/>
-      <c s="36" r="R35"/>
-      <c s="36" r="S35"/>
-      <c t="str" s="33" r="T35">
+      <c s="37" r="P35"/>
+      <c s="37" r="Q35"/>
+      <c s="37" r="R35"/>
+      <c s="37" r="S35"/>
+      <c t="str" s="34" r="T35">
         <f>SUM(H35:S35)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U35"/>
+      <c s="32" r="U35"/>
     </row>
     <row r="36">
-      <c s="18" r="A36">
+      <c s="19" r="A36">
         <v>34.0</v>
       </c>
-      <c t="s" s="24" r="B36">
+      <c t="s" s="25" r="B36">
         <v>145</v>
       </c>
-      <c t="s" s="25" r="E36">
+      <c t="s" s="26" r="E36">
         <v>146</v>
       </c>
-      <c s="39" r="F36">
+      <c s="40" r="F36">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G36">
+      <c t="s" s="42" r="G36">
         <v>147</v>
       </c>
-      <c s="28" r="H36"/>
-      <c s="28" r="I36"/>
-      <c s="28" r="J36"/>
-      <c t="s" s="29" r="K36">
+      <c s="29" r="H36"/>
+      <c s="29" r="I36"/>
+      <c s="29" r="J36"/>
+      <c t="s" s="30" r="K36">
         <v>148</v>
       </c>
-      <c t="s" s="29" r="L36">
+      <c t="s" s="30" r="L36">
         <v>149</v>
       </c>
-      <c s="28" r="M36"/>
-      <c s="28" r="N36"/>
-      <c s="27" r="O36">
+      <c s="29" r="M36"/>
+      <c s="29" r="N36"/>
+      <c s="28" r="O36">
         <v>8.0</v>
       </c>
-      <c s="28" r="P36"/>
-      <c s="28" r="Q36"/>
-      <c s="28" r="R36"/>
-      <c s="28" r="S36"/>
-      <c t="str" s="33" r="T36">
+      <c s="29" r="P36"/>
+      <c s="29" r="Q36"/>
+      <c s="29" r="R36"/>
+      <c s="29" r="S36"/>
+      <c t="str" s="34" r="T36">
         <f>SUM(H36:S36)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U36"/>
+      <c s="32" r="U36"/>
     </row>
     <row r="37">
-      <c s="18" r="A37">
+      <c s="19" r="A37">
         <v>35.0</v>
       </c>
-      <c t="s" s="24" r="B37">
+      <c t="s" s="25" r="B37">
         <v>150</v>
       </c>
-      <c t="s" s="25" r="E37">
+      <c t="s" s="26" r="E37">
         <v>151</v>
       </c>
-      <c s="39" r="F37">
+      <c s="40" r="F37">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G37">
+      <c t="s" s="42" r="G37">
         <v>152</v>
       </c>
-      <c s="37" r="H37"/>
-      <c s="37" r="I37"/>
-      <c s="37" r="J37"/>
-      <c t="s" s="29" r="K37">
+      <c s="38" r="H37"/>
+      <c s="38" r="I37"/>
+      <c s="38" r="J37"/>
+      <c t="s" s="30" r="K37">
         <v>153</v>
       </c>
-      <c t="s" s="29" r="L37">
+      <c t="s" s="30" r="L37">
         <v>154</v>
       </c>
-      <c s="37" r="M37"/>
-      <c s="37" r="N37"/>
-      <c s="38" r="O37">
+      <c s="38" r="M37"/>
+      <c s="38" r="N37"/>
+      <c s="39" r="O37">
         <v>8.0</v>
       </c>
-      <c s="37" r="P37"/>
-      <c s="37" r="Q37"/>
-      <c s="37" r="R37"/>
-      <c s="37" r="S37"/>
-      <c t="str" s="33" r="T37">
+      <c s="38" r="P37"/>
+      <c s="38" r="Q37"/>
+      <c s="38" r="R37"/>
+      <c s="38" r="S37"/>
+      <c t="str" s="34" r="T37">
         <f>SUM(H37:S37)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U37"/>
+      <c s="32" r="U37"/>
     </row>
     <row r="38">
-      <c s="18" r="A38">
+      <c s="19" r="A38">
         <v>37.0</v>
       </c>
-      <c t="s" s="24" r="B38">
+      <c t="s" s="25" r="B38">
         <v>155</v>
       </c>
-      <c s="25" r="E38">
+      <c s="26" r="E38">
         <v>25.0</v>
       </c>
-      <c s="39" r="F38">
+      <c s="40" r="F38">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G38">
+      <c t="s" s="42" r="G38">
         <v>156</v>
       </c>
-      <c s="37" r="H38"/>
-      <c s="37" r="I38"/>
-      <c s="37" r="J38"/>
-      <c t="s" s="29" r="K38">
+      <c s="38" r="H38"/>
+      <c s="38" r="I38"/>
+      <c s="38" r="J38"/>
+      <c t="s" s="30" r="K38">
         <v>157</v>
       </c>
-      <c t="s" s="29" r="L38">
+      <c t="s" s="30" r="L38">
         <v>158</v>
       </c>
-      <c s="37" r="M38"/>
-      <c s="37" r="N38"/>
-      <c s="38" r="O38">
+      <c s="38" r="M38"/>
+      <c s="38" r="N38"/>
+      <c s="39" r="O38">
         <v>8.0</v>
       </c>
-      <c s="37" r="P38"/>
-      <c s="37" r="Q38"/>
-      <c s="37" r="R38"/>
-      <c s="37" r="S38"/>
-      <c t="str" s="33" r="T38">
+      <c s="38" r="P38"/>
+      <c s="38" r="Q38"/>
+      <c s="38" r="R38"/>
+      <c s="38" r="S38"/>
+      <c t="str" s="34" r="T38">
         <f>SUM(H38:S38)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U38"/>
+      <c s="32" r="U38"/>
     </row>
     <row r="39">
-      <c s="18" r="A39">
+      <c s="19" r="A39">
         <v>38.0</v>
       </c>
-      <c t="s" s="24" r="B39">
+      <c t="s" s="25" r="B39">
         <v>159</v>
       </c>
-      <c s="25" r="E39">
+      <c s="26" r="E39">
         <v>31.0</v>
       </c>
-      <c s="39" r="F39">
+      <c s="40" r="F39">
         <v>32.0</v>
       </c>
-      <c t="s" s="32" r="G39">
+      <c t="s" s="33" r="G39">
         <v>160</v>
       </c>
-      <c s="28" r="H39"/>
-      <c s="28" r="I39"/>
-      <c s="28" r="J39"/>
-      <c t="s" s="29" r="K39">
+      <c s="29" r="H39"/>
+      <c s="29" r="I39"/>
+      <c s="29" r="J39"/>
+      <c t="s" s="30" r="K39">
         <v>161</v>
       </c>
-      <c t="s" s="29" r="L39">
+      <c t="s" s="30" r="L39">
         <v>162</v>
       </c>
-      <c s="28" r="M39"/>
-      <c s="28" r="N39"/>
-      <c s="28" r="O39"/>
-      <c s="27" r="P39">
+      <c s="29" r="M39"/>
+      <c s="29" r="N39"/>
+      <c s="29" r="O39"/>
+      <c s="28" r="P39">
         <v>20.0</v>
       </c>
-      <c s="27" r="Q39">
+      <c s="28" r="Q39">
         <v>12.0</v>
       </c>
-      <c s="28" r="R39"/>
-      <c s="28" r="S39"/>
-      <c t="str" s="33" r="T39">
+      <c s="29" r="R39"/>
+      <c s="29" r="S39"/>
+      <c t="str" s="34" r="T39">
         <f>SUM(H39:S39)</f>
         <v>32</v>
       </c>
-      <c s="31" r="U39"/>
+      <c s="32" r="U39"/>
     </row>
     <row r="40">
-      <c s="18" r="A40">
+      <c s="19" r="A40">
         <v>39.0</v>
       </c>
-      <c t="s" s="24" r="B40">
+      <c t="s" s="25" r="B40">
         <v>163</v>
       </c>
-      <c s="25" r="E40">
+      <c s="26" r="E40">
         <v>31.0</v>
       </c>
-      <c s="39" r="F40">
+      <c s="40" r="F40">
         <v>24.0</v>
       </c>
-      <c t="s" s="32" r="G40">
+      <c t="s" s="33" r="G40">
         <v>164</v>
       </c>
-      <c s="28" r="H40"/>
-      <c s="28" r="I40"/>
-      <c s="28" r="J40"/>
-      <c t="s" s="29" r="K40">
+      <c s="29" r="H40"/>
+      <c s="29" r="I40"/>
+      <c s="29" r="J40"/>
+      <c t="s" s="30" r="K40">
         <v>165</v>
       </c>
-      <c t="s" s="29" r="L40">
+      <c t="s" s="30" r="L40">
         <v>166</v>
       </c>
-      <c s="28" r="M40"/>
-      <c s="28" r="N40"/>
-      <c s="28" r="O40"/>
-      <c s="27" r="P40">
+      <c s="29" r="M40"/>
+      <c s="29" r="N40"/>
+      <c s="29" r="O40"/>
+      <c s="28" r="P40">
         <v>24.0</v>
       </c>
-      <c s="28" r="Q40"/>
-      <c s="28" r="R40"/>
-      <c s="28" r="S40"/>
-      <c t="str" s="33" r="T40">
+      <c s="29" r="Q40"/>
+      <c s="29" r="R40"/>
+      <c s="29" r="S40"/>
+      <c t="str" s="34" r="T40">
         <f>SUM(H40:S40)</f>
         <v>24</v>
       </c>
-      <c s="31" r="U40"/>
+      <c s="32" r="U40"/>
     </row>
     <row r="41">
-      <c s="18" r="A41">
+      <c s="19" r="A41">
         <v>40.0</v>
       </c>
-      <c t="s" s="24" r="B41">
+      <c t="s" s="25" r="B41">
         <v>167</v>
       </c>
-      <c s="25" r="E41">
+      <c s="26" r="E41">
         <v>32.0</v>
       </c>
-      <c s="39" r="F41">
+      <c s="40" r="F41">
         <v>16.0</v>
       </c>
-      <c t="s" s="32" r="G41">
+      <c t="s" s="33" r="G41">
         <v>168</v>
       </c>
-      <c s="28" r="H41"/>
-      <c s="28" r="I41"/>
-      <c s="28" r="J41"/>
-      <c t="s" s="29" r="K41">
+      <c s="29" r="H41"/>
+      <c s="29" r="I41"/>
+      <c s="29" r="J41"/>
+      <c t="s" s="30" r="K41">
         <v>169</v>
       </c>
-      <c t="s" s="29" r="L41">
+      <c t="s" s="30" r="L41">
         <v>170</v>
       </c>
-      <c s="28" r="M41"/>
-      <c s="28" r="N41"/>
-      <c s="28" r="O41"/>
-      <c s="27" r="P41"/>
-      <c s="27" r="Q41">
+      <c s="29" r="M41"/>
+      <c s="29" r="N41"/>
+      <c s="29" r="O41"/>
+      <c s="28" r="P41"/>
+      <c s="28" r="Q41">
         <v>8.0</v>
       </c>
-      <c s="27" r="R41">
+      <c s="28" r="R41">
         <v>8.0</v>
       </c>
-      <c s="27" r="S41"/>
-      <c t="str" s="33" r="T41">
+      <c s="28" r="S41"/>
+      <c t="str" s="34" r="T41">
         <f>SUM(H41:S41)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U41"/>
+      <c s="32" r="U41"/>
     </row>
     <row r="42">
-      <c s="18" r="A42">
+      <c s="19" r="A42">
         <v>41.0</v>
       </c>
-      <c t="s" s="24" r="B42">
+      <c t="s" s="25" r="B42">
         <v>171</v>
       </c>
-      <c s="25" r="E42">
+      <c s="26" r="E42">
         <v>33.0</v>
       </c>
-      <c s="44" r="F42">
+      <c s="45" r="F42">
         <v>16.0</v>
       </c>
-      <c t="s" s="41" r="G42">
+      <c t="s" s="42" r="G42">
         <v>172</v>
       </c>
-      <c s="28" r="H42"/>
-      <c s="28" r="I42"/>
-      <c s="28" r="J42"/>
-      <c t="s" s="29" r="K42">
+      <c s="29" r="H42"/>
+      <c s="29" r="I42"/>
+      <c s="29" r="J42"/>
+      <c t="s" s="30" r="K42">
         <v>173</v>
       </c>
-      <c t="s" s="29" r="L42">
+      <c t="s" s="30" r="L42">
         <v>174</v>
       </c>
-      <c s="28" r="M42"/>
-      <c s="28" r="N42"/>
-      <c s="28" r="O42"/>
-      <c s="27" r="P42">
+      <c s="29" r="M42"/>
+      <c s="29" r="N42"/>
+      <c s="29" r="O42"/>
+      <c s="28" r="P42">
         <v>16.0</v>
       </c>
-      <c s="28" r="Q42"/>
-      <c s="28" r="R42"/>
-      <c s="28" r="S42"/>
-      <c t="str" s="33" r="T42">
+      <c s="29" r="Q42"/>
+      <c s="29" r="R42"/>
+      <c s="29" r="S42"/>
+      <c t="str" s="34" r="T42">
         <f>SUM(H42:S42)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U42"/>
+      <c s="32" r="U42"/>
     </row>
     <row r="43">
-      <c s="18" r="A43">
+      <c s="19" r="A43">
         <v>42.0</v>
       </c>
-      <c t="s" s="24" r="B43">
+      <c t="s" s="25" r="B43">
         <v>175</v>
       </c>
-      <c t="s" s="25" r="E43">
+      <c t="s" s="26" r="E43">
         <v>176</v>
       </c>
-      <c s="39" r="F43">
+      <c s="40" r="F43">
         <v>16.0</v>
       </c>
-      <c t="s" s="32" r="G43">
+      <c t="s" s="33" r="G43">
         <v>177</v>
       </c>
-      <c s="28" r="H43"/>
-      <c s="28" r="I43"/>
-      <c s="28" r="J43"/>
-      <c t="s" s="29" r="K43">
+      <c s="29" r="H43"/>
+      <c s="29" r="I43"/>
+      <c s="29" r="J43"/>
+      <c t="s" s="30" r="K43">
         <v>178</v>
       </c>
-      <c t="s" s="29" r="L43">
+      <c t="s" s="30" r="L43">
         <v>179</v>
       </c>
-      <c s="28" r="M43"/>
-      <c s="28" r="N43"/>
-      <c s="28" r="O43"/>
-      <c s="27" r="P43">
+      <c s="29" r="M43"/>
+      <c s="29" r="N43"/>
+      <c s="29" r="O43"/>
+      <c s="28" r="P43">
         <v>5.0</v>
       </c>
-      <c s="27" r="Q43">
+      <c s="28" r="Q43">
         <v>11.0</v>
       </c>
-      <c s="28" r="R43"/>
-      <c s="28" r="S43"/>
-      <c t="str" s="33" r="T43">
+      <c s="29" r="R43"/>
+      <c s="29" r="S43"/>
+      <c t="str" s="34" r="T43">
         <f>SUM(H43:S43)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U43"/>
+      <c s="32" r="U43"/>
     </row>
     <row r="44">
-      <c s="18" r="A44">
+      <c s="19" r="A44">
         <v>43.0</v>
       </c>
-      <c t="s" s="24" r="B44">
+      <c t="s" s="25" r="B44">
         <v>180</v>
       </c>
-      <c t="s" s="25" r="E44">
+      <c t="s" s="26" r="E44">
         <v>181</v>
       </c>
-      <c s="39" r="F44">
+      <c s="40" r="F44">
         <v>16.0</v>
       </c>
-      <c t="s" s="32" r="G44">
+      <c t="s" s="33" r="G44">
         <v>182</v>
       </c>
-      <c s="28" r="H44"/>
-      <c s="28" r="I44"/>
-      <c s="28" r="J44"/>
-      <c t="s" s="29" r="K44">
+      <c s="29" r="H44"/>
+      <c s="29" r="I44"/>
+      <c s="29" r="J44"/>
+      <c t="s" s="30" r="K44">
         <v>183</v>
       </c>
-      <c t="s" s="29" r="L44">
+      <c t="s" s="30" r="L44">
         <v>184</v>
       </c>
-      <c s="28" r="M44"/>
-      <c s="28" r="N44"/>
-      <c s="28" r="O44"/>
-      <c s="27" r="P44"/>
-      <c s="27" r="Q44">
+      <c s="29" r="M44"/>
+      <c s="29" r="N44"/>
+      <c s="29" r="O44"/>
+      <c s="28" r="P44"/>
+      <c s="28" r="Q44">
         <v>16.0</v>
       </c>
-      <c s="28" r="R44"/>
-      <c s="28" r="S44"/>
-      <c t="str" s="33" r="T44">
+      <c s="29" r="R44"/>
+      <c s="29" r="S44"/>
+      <c t="str" s="34" r="T44">
         <f>SUM(H44:S44)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U44"/>
+      <c s="32" r="U44"/>
     </row>
     <row r="45">
-      <c s="18" r="A45">
+      <c s="19" r="A45">
         <v>44.0</v>
       </c>
-      <c t="s" s="24" r="B45">
+      <c t="s" s="25" r="B45">
         <v>185</v>
       </c>
-      <c t="s" s="25" r="E45">
+      <c t="s" s="26" r="E45">
         <v>186</v>
       </c>
-      <c s="44" r="F45">
+      <c s="45" r="F45">
         <v>16.0</v>
       </c>
-      <c t="s" s="40" r="G45">
+      <c t="s" s="41" r="G45">
         <v>187</v>
       </c>
-      <c s="45" r="H45"/>
-      <c s="45" r="I45"/>
-      <c s="45" r="J45"/>
-      <c t="s" s="29" r="K45">
+      <c s="46" r="H45"/>
+      <c s="46" r="I45"/>
+      <c s="46" r="J45"/>
+      <c t="s" s="30" r="K45">
         <v>188</v>
       </c>
-      <c t="s" s="29" r="L45">
+      <c t="s" s="30" r="L45">
         <v>189</v>
       </c>
-      <c s="45" r="M45"/>
-      <c s="45" r="N45"/>
-      <c s="45" r="O45"/>
-      <c s="34" r="P45"/>
-      <c s="34" r="Q45">
+      <c s="46" r="M45"/>
+      <c s="46" r="N45"/>
+      <c s="46" r="O45"/>
+      <c s="35" r="P45"/>
+      <c s="35" r="Q45">
         <v>16.0</v>
       </c>
-      <c s="45" r="R45"/>
-      <c s="45" r="S45"/>
-      <c t="str" s="33" r="T45">
+      <c s="46" r="R45"/>
+      <c s="46" r="S45"/>
+      <c t="str" s="34" r="T45">
         <f>SUM(H45:S45)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U45"/>
+      <c s="32" r="U45"/>
     </row>
     <row customHeight="1" r="46" ht="18.0">
-      <c s="18" r="A46">
+      <c s="19" r="A46">
         <v>45.0</v>
       </c>
-      <c t="s" s="24" r="B46">
+      <c t="s" s="25" r="B46">
         <v>190</v>
       </c>
-      <c t="s" s="25" r="E46">
+      <c t="s" s="26" r="E46">
         <v>191</v>
       </c>
-      <c s="39" r="F46">
+      <c s="40" r="F46">
         <v>16.0</v>
       </c>
-      <c t="s" s="41" r="G46">
+      <c t="s" s="42" r="G46">
         <v>192</v>
       </c>
-      <c s="28" r="H46"/>
-      <c s="28" r="I46"/>
-      <c s="28" r="J46"/>
-      <c t="s" s="29" r="K46">
+      <c s="29" r="H46"/>
+      <c s="29" r="I46"/>
+      <c s="29" r="J46"/>
+      <c t="s" s="30" r="K46">
         <v>193</v>
       </c>
-      <c t="s" s="29" r="L46">
+      <c t="s" s="30" r="L46">
         <v>194</v>
       </c>
-      <c s="28" r="M46"/>
-      <c s="28" r="N46"/>
-      <c s="28" r="O46"/>
-      <c s="27" r="P46"/>
-      <c s="27" r="Q46">
+      <c s="29" r="M46"/>
+      <c s="29" r="N46"/>
+      <c s="29" r="O46"/>
+      <c s="28" r="P46"/>
+      <c s="28" r="Q46">
         <v>16.0</v>
       </c>
-      <c s="28" r="R46"/>
-      <c s="28" r="S46"/>
-      <c t="str" s="33" r="T46">
+      <c s="29" r="R46"/>
+      <c s="29" r="S46"/>
+      <c t="str" s="34" r="T46">
         <f>SUM(H46:S46)</f>
         <v>16</v>
       </c>
-      <c s="31" r="U46"/>
+      <c s="32" r="U46"/>
     </row>
     <row r="47">
-      <c s="18" r="A47">
+      <c s="19" r="A47">
         <v>46.0</v>
       </c>
-      <c t="s" s="24" r="B47">
+      <c t="s" s="25" r="B47">
         <v>195</v>
       </c>
-      <c t="s" s="25" r="E47">
+      <c t="s" s="26" r="E47">
         <v>196</v>
       </c>
-      <c s="39" r="F47">
+      <c s="40" r="F47">
         <v>40.0</v>
       </c>
-      <c t="s" s="41" r="G47">
+      <c t="s" s="42" r="G47">
         <v>197</v>
       </c>
-      <c s="28" r="H47"/>
-      <c s="28" r="I47"/>
-      <c s="28" r="J47"/>
-      <c t="s" s="29" r="K47">
+      <c s="29" r="H47"/>
+      <c s="29" r="I47"/>
+      <c s="29" r="J47"/>
+      <c t="s" s="30" r="K47">
         <v>198</v>
       </c>
-      <c t="s" s="29" r="L47">
+      <c t="s" s="30" r="L47">
         <v>199</v>
       </c>
-      <c s="28" r="M47"/>
-      <c s="28" r="N47"/>
-      <c s="28" r="O47"/>
-      <c s="27" r="P47">
+      <c s="29" r="M47"/>
+      <c s="29" r="N47"/>
+      <c s="29" r="O47"/>
+      <c s="28" r="P47">
         <v>40.0</v>
       </c>
-      <c s="27" r="Q47"/>
-      <c s="27" r="R47"/>
-      <c s="28" r="S47"/>
-      <c t="str" s="33" r="T47">
+      <c s="28" r="Q47"/>
+      <c s="28" r="R47"/>
+      <c s="29" r="S47"/>
+      <c t="str" s="34" r="T47">
         <f>SUM(H47:S47)</f>
         <v>40</v>
       </c>
-      <c s="31" r="U47"/>
+      <c s="32" r="U47"/>
     </row>
     <row r="48">
-      <c s="18" r="A48">
+      <c s="19" r="A48">
         <v>47.0</v>
       </c>
-      <c t="s" s="24" r="B48">
+      <c t="s" s="25" r="B48">
         <v>200</v>
       </c>
-      <c t="s" s="25" r="E48">
+      <c t="s" s="26" r="E48">
         <v>201</v>
       </c>
-      <c s="39" r="F48">
+      <c s="40" r="F48">
         <v>40.0</v>
       </c>
-      <c t="s" s="41" r="G48">
+      <c t="s" s="42" r="G48">
         <v>202</v>
       </c>
-      <c s="28" r="H48"/>
-      <c s="28" r="I48"/>
-      <c s="28" r="J48"/>
-      <c t="s" s="29" r="K48">
+      <c s="29" r="H48"/>
+      <c s="29" r="I48"/>
+      <c s="29" r="J48"/>
+      <c t="s" s="30" r="K48">
         <v>203</v>
       </c>
-      <c t="s" s="29" r="L48">
+      <c t="s" s="30" r="L48">
         <v>204</v>
       </c>
-      <c s="28" r="M48"/>
-      <c s="28" r="N48"/>
-      <c s="28" r="O48"/>
-      <c s="28" r="P48"/>
-      <c s="28" r="Q48"/>
-      <c s="27" r="R48">
+      <c s="29" r="M48"/>
+      <c s="29" r="N48"/>
+      <c s="29" r="O48"/>
+      <c s="29" r="P48"/>
+      <c s="29" r="Q48"/>
+      <c s="28" r="R48">
         <v>8.0</v>
       </c>
-      <c s="27" r="S48">
+      <c s="28" r="S48">
         <v>32.0</v>
       </c>
-      <c t="str" s="33" r="T48">
+      <c t="str" s="34" r="T48">
         <f>SUM(H48:S48)</f>
         <v>40</v>
       </c>
-      <c s="31" r="U48"/>
+      <c s="32" r="U48"/>
     </row>
     <row customHeight="1" r="49" ht="1.5">
-      <c s="18" r="A49">
+      <c s="19" r="A49">
         <v>48.0</v>
       </c>
-      <c t="s" s="24" r="B49">
+      <c t="s" s="25" r="B49">
         <v>205</v>
       </c>
-      <c s="25" r="E49"/>
-      <c s="39" r="F49">
+      <c s="26" r="E49"/>
+      <c s="40" r="F49">
         <v>72.0</v>
       </c>
-      <c t="s" s="41" r="G49">
+      <c t="s" s="42" r="G49">
         <v>206</v>
       </c>
-      <c s="28" r="H49"/>
-      <c s="28" r="I49"/>
-      <c s="28" r="J49"/>
-      <c t="s" s="29" r="K49">
+      <c s="29" r="H49"/>
+      <c s="29" r="I49"/>
+      <c s="29" r="J49"/>
+      <c t="s" s="30" r="K49">
         <v>207</v>
       </c>
-      <c t="s" s="29" r="L49">
+      <c t="s" s="30" r="L49">
         <v>208</v>
       </c>
-      <c s="27" r="M49">
+      <c s="28" r="M49">
         <v>10.0</v>
       </c>
-      <c s="27" r="N49">
+      <c s="28" r="N49">
         <v>10.0</v>
       </c>
-      <c s="27" r="O49">
+      <c s="28" r="O49">
         <v>10.0</v>
       </c>
-      <c s="27" r="P49">
+      <c s="28" r="P49">
         <v>10.0</v>
       </c>
-      <c s="27" r="Q49">
+      <c s="28" r="Q49">
         <v>10.0</v>
       </c>
-      <c s="27" r="R49">
+      <c s="28" r="R49">
         <v>10.0</v>
       </c>
-      <c s="27" r="S49">
+      <c s="28" r="S49">
         <v>12.0</v>
       </c>
-      <c t="str" s="33" r="T49">
+      <c t="str" s="34" r="T49">
         <f>SUM(H49:S49)</f>
         <v>72</v>
       </c>
-      <c s="31" r="U49"/>
+      <c s="32" r="U49"/>
     </row>
     <row r="50">
-      <c s="18" r="A50">
+      <c s="19" r="A50">
         <v>49.0</v>
       </c>
-      <c t="s" s="24" r="B50">
+      <c t="s" s="25" r="B50">
         <v>209</v>
       </c>
-      <c s="25" r="E50"/>
-      <c s="39" r="F50">
+      <c s="26" r="E50"/>
+      <c s="40" r="F50">
         <v>32.0</v>
       </c>
-      <c t="s" s="41" r="G50">
+      <c t="s" s="42" r="G50">
         <v>210</v>
       </c>
-      <c s="28" r="H50"/>
-      <c s="28" r="I50"/>
-      <c s="28" r="J50"/>
-      <c t="s" s="29" r="K50">
+      <c s="29" r="H50"/>
+      <c s="29" r="I50"/>
+      <c s="29" r="J50"/>
+      <c t="s" s="30" r="K50">
         <v>211</v>
       </c>
-      <c t="s" s="29" r="L50">
+      <c t="s" s="30" r="L50">
         <v>212</v>
       </c>
-      <c s="28" r="M50"/>
-      <c s="27" r="N50"/>
-      <c s="27" r="O50"/>
-      <c s="27" r="P50"/>
-      <c s="27" r="Q50">
+      <c s="29" r="M50"/>
+      <c s="28" r="N50"/>
+      <c s="28" r="O50"/>
+      <c s="28" r="P50"/>
+      <c s="28" r="Q50">
         <v>8.0</v>
       </c>
-      <c s="27" r="R50">
+      <c s="28" r="R50">
         <v>24.0</v>
       </c>
-      <c s="28" r="S50"/>
-      <c t="str" s="33" r="T50">
+      <c s="29" r="S50"/>
+      <c t="str" s="34" r="T50">
         <f>SUM(H50:S50)</f>
         <v>32</v>
       </c>
-      <c s="31" r="U50"/>
+      <c s="32" r="U50"/>
     </row>
     <row r="51">
-      <c s="18" r="A51">
+      <c s="19" r="A51">
         <v>50.0</v>
       </c>
-      <c t="s" s="24" r="B51">
+      <c t="s" s="25" r="B51">
         <v>213</v>
       </c>
-      <c s="25" r="E51"/>
-      <c s="39" r="F51">
+      <c s="26" r="E51"/>
+      <c s="40" r="F51">
         <v>10.0</v>
       </c>
-      <c t="s" s="41" r="G51">
+      <c t="s" s="42" r="G51">
         <v>214</v>
       </c>
-      <c s="27" r="H51">
+      <c s="28" r="H51">
         <v>1.0</v>
       </c>
-      <c s="27" r="I51">
+      <c s="28" r="I51">
         <v>1.0</v>
       </c>
-      <c s="27" r="J51">
+      <c s="28" r="J51">
         <v>1.0</v>
       </c>
-      <c t="s" s="29" r="K51">
+      <c t="s" s="30" r="K51">
         <v>215</v>
       </c>
-      <c t="s" s="29" r="L51">
+      <c t="s" s="30" r="L51">
         <v>216</v>
       </c>
-      <c s="27" r="M51">
+      <c s="28" r="M51">
         <v>1.0</v>
       </c>
-      <c s="27" r="N51">
+      <c s="28" r="N51">
         <v>1.0</v>
       </c>
-      <c s="27" r="O51">
+      <c s="28" r="O51">
         <v>1.0</v>
       </c>
-      <c s="27" r="P51">
+      <c s="28" r="P51">
         <v>1.0</v>
       </c>
-      <c s="27" r="Q51">
+      <c s="28" r="Q51">
         <v>1.0</v>
       </c>
-      <c s="27" r="R51">
+      <c s="28" r="R51">
         <v>1.0</v>
       </c>
-      <c s="27" r="S51">
+      <c s="28" r="S51">
         <v>1.0</v>
       </c>
-      <c t="str" s="33" r="T51">
+      <c t="str" s="34" r="T51">
         <f>SUM(H51:S51)</f>
         <v>10</v>
       </c>
-      <c s="31" r="U51"/>
+      <c s="32" r="U51"/>
     </row>
     <row r="52">
-      <c s="18" r="A52">
+      <c s="19" r="A52">
         <v>51.0</v>
       </c>
-      <c t="s" s="24" r="B52">
+      <c t="s" s="25" r="B52">
         <v>217</v>
       </c>
-      <c s="25" r="E52"/>
-      <c s="39" r="F52">
+      <c s="26" r="E52"/>
+      <c s="40" r="F52">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G52">
+      <c t="s" s="42" r="G52">
         <v>218</v>
       </c>
-      <c s="28" r="H52"/>
-      <c s="28" r="I52"/>
-      <c s="28" r="J52"/>
-      <c t="s" s="29" r="K52">
+      <c s="29" r="H52"/>
+      <c s="29" r="I52"/>
+      <c s="29" r="J52"/>
+      <c t="s" s="30" r="K52">
         <v>219</v>
       </c>
-      <c t="s" s="29" r="L52">
+      <c t="s" s="30" r="L52">
         <v>220</v>
       </c>
-      <c s="28" r="M52"/>
-      <c s="28" r="N52"/>
-      <c s="28" r="O52"/>
-      <c s="28" r="P52"/>
-      <c s="28" r="Q52"/>
-      <c s="28" r="R52"/>
-      <c s="27" r="S52">
+      <c s="29" r="M52"/>
+      <c s="29" r="N52"/>
+      <c s="29" r="O52"/>
+      <c s="29" r="P52"/>
+      <c s="29" r="Q52"/>
+      <c s="29" r="R52"/>
+      <c s="28" r="S52">
         <v>8.0</v>
       </c>
-      <c t="str" s="33" r="T52">
+      <c t="str" s="34" r="T52">
         <f>SUM(H52:S52)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U52"/>
+      <c s="32" r="U52"/>
     </row>
     <row r="53">
-      <c s="18" r="A53">
+      <c s="19" r="A53">
         <v>52.0</v>
       </c>
-      <c t="s" s="24" r="B53">
+      <c t="s" s="25" r="B53">
         <v>221</v>
       </c>
-      <c s="25" r="E53"/>
-      <c s="39" r="F53">
+      <c s="26" r="E53"/>
+      <c s="40" r="F53">
         <v>8.0</v>
       </c>
-      <c t="s" s="41" r="G53">
+      <c t="s" s="42" r="G53">
         <v>222</v>
       </c>
-      <c s="28" r="H53"/>
-      <c s="28" r="I53"/>
-      <c s="28" r="J53"/>
-      <c t="s" s="29" r="K53">
+      <c s="29" r="H53"/>
+      <c s="29" r="I53"/>
+      <c s="29" r="J53"/>
+      <c t="s" s="30" r="K53">
         <v>223</v>
       </c>
-      <c t="s" s="29" r="L53">
+      <c t="s" s="30" r="L53">
         <v>224</v>
       </c>
-      <c s="28" r="M53"/>
-      <c s="28" r="N53"/>
-      <c s="28" r="O53"/>
-      <c s="28" r="P53"/>
-      <c s="28" r="Q53"/>
-      <c s="28" r="R53"/>
-      <c s="27" r="S53">
+      <c s="29" r="M53"/>
+      <c s="29" r="N53"/>
+      <c s="29" r="O53"/>
+      <c s="29" r="P53"/>
+      <c s="29" r="Q53"/>
+      <c s="29" r="R53"/>
+      <c s="28" r="S53">
         <v>8.0</v>
       </c>
-      <c t="str" s="33" r="T53">
+      <c t="str" s="34" r="T53">
         <f>SUM(H53:S53)</f>
         <v>8</v>
       </c>
-      <c s="31" r="U53"/>
+      <c s="32" r="U53"/>
     </row>
     <row r="54">
-      <c s="18" r="A54">
+      <c s="19" r="A54">
         <v>53.0</v>
       </c>
-      <c t="s" s="24" r="B54">
+      <c t="s" s="25" r="B54">
         <v>225</v>
       </c>
-      <c s="46" r="E54"/>
-      <c s="39" r="F54">
+      <c s="47" r="E54"/>
+      <c s="40" r="F54">
         <v>32.0</v>
       </c>
-      <c t="s" s="41" r="G54">
+      <c t="s" s="42" r="G54">
         <v>226</v>
       </c>
-      <c s="28" r="H54"/>
-      <c s="28" r="I54"/>
-      <c s="28" r="J54"/>
-      <c t="s" s="29" r="K54">
+      <c s="29" r="H54"/>
+      <c s="29" r="I54"/>
+      <c s="29" r="J54"/>
+      <c t="s" s="30" r="K54">
         <v>227</v>
       </c>
-      <c t="s" s="29" r="L54">
+      <c t="s" s="30" r="L54">
         <v>228</v>
       </c>
-      <c s="28" r="M54"/>
-      <c s="28" r="N54"/>
-      <c s="28" r="O54"/>
-      <c s="28" r="P54"/>
-      <c s="28" r="Q54"/>
-      <c s="28" r="R54"/>
-      <c s="27" r="S54">
+      <c s="29" r="M54"/>
+      <c s="29" r="N54"/>
+      <c s="29" r="O54"/>
+      <c s="29" r="P54"/>
+      <c s="29" r="Q54"/>
+      <c s="29" r="R54"/>
+      <c s="28" r="S54">
         <v>32.0</v>
       </c>
-      <c t="str" s="33" r="T54">
+      <c t="str" s="34" r="T54">
         <f>SUM(H54:S54)</f>
         <v>32</v>
       </c>
-      <c s="31" r="U54"/>
+      <c s="32" r="U54"/>
     </row>
     <row r="55">
-      <c s="18" r="A55">
+      <c s="19" r="A55">
         <v>54.0</v>
       </c>
-      <c t="s" s="24" r="B55">
+      <c t="s" s="25" r="B55">
         <v>229</v>
       </c>
-      <c s="46" r="E55"/>
-      <c s="39" r="F55">
+      <c s="47" r="E55"/>
+      <c s="40" r="F55">
         <v>3.0</v>
       </c>
-      <c t="s" s="41" r="G55">
+      <c t="s" s="42" r="G55">
         <v>230</v>
       </c>
-      <c s="28" r="H55"/>
-      <c s="28" r="I55"/>
-      <c s="28" r="J55"/>
-      <c t="s" s="29" r="K55">
+      <c s="29" r="H55"/>
+      <c s="29" r="I55"/>
+      <c s="29" r="J55"/>
+      <c t="s" s="30" r="K55">
         <v>231</v>
       </c>
-      <c t="s" s="29" r="L55">
+      <c t="s" s="30" r="L55">
         <v>232</v>
       </c>
-      <c s="27" r="M55">
+      <c s="28" r="M55">
         <v>1.0</v>
       </c>
-      <c s="27" r="N55">
+      <c s="28" r="N55">
         <v>1.0</v>
       </c>
-      <c s="27" r="O55">
+      <c s="28" r="O55">
         <v>1.0</v>
       </c>
-      <c s="28" r="P55"/>
-      <c s="28" r="Q55"/>
-      <c s="28" r="R55"/>
-      <c s="28" r="S55"/>
-      <c t="str" s="33" r="T55">
+      <c s="29" r="P55"/>
+      <c s="29" r="Q55"/>
+      <c s="29" r="R55"/>
+      <c s="29" r="S55"/>
+      <c t="str" s="34" r="T55">
         <f>SUM(H55:S55)</f>
         <v>3</v>
       </c>
-      <c s="31" r="U55"/>
+      <c s="32" r="U55"/>
     </row>
     <row r="56">
-      <c s="18" r="A56">
+      <c s="19" r="A56">
         <v>55.0</v>
       </c>
-      <c t="s" s="24" r="B56">
+      <c t="s" s="25" r="B56">
         <v>233</v>
       </c>
-      <c s="46" r="E56"/>
-      <c s="44" r="F56">
+      <c s="47" r="E56"/>
+      <c s="45" r="F56">
         <v>100.0</v>
       </c>
-      <c t="s" s="43" r="G56">
+      <c t="s" s="44" r="G56">
         <v>234</v>
       </c>
-      <c s="34" r="H56">
+      <c s="35" r="H56">
         <v>33.0</v>
       </c>
-      <c s="34" r="I56">
+      <c s="35" r="I56">
         <v>34.0</v>
       </c>
-      <c s="34" r="J56">
+      <c s="35" r="J56">
         <v>33.0</v>
       </c>
-      <c t="s" s="47" r="K56">
+      <c t="s" s="48" r="K56">
         <v>235</v>
       </c>
-      <c t="s" s="47" r="L56">
+      <c t="s" s="48" r="L56">
         <v>236</v>
       </c>
-      <c s="45" r="M56"/>
-      <c s="45" r="N56"/>
-      <c s="45" r="O56"/>
-      <c s="45" r="P56"/>
-      <c s="45" r="Q56"/>
-      <c s="45" r="R56"/>
-      <c s="48" r="S56"/>
-      <c t="str" s="33" r="T56">
+      <c s="46" r="M56"/>
+      <c s="46" r="N56"/>
+      <c s="46" r="O56"/>
+      <c s="46" r="P56"/>
+      <c s="46" r="Q56"/>
+      <c s="46" r="R56"/>
+      <c s="49" r="S56"/>
+      <c t="str" s="34" r="T56">
         <f>SUM(H56:S56)</f>
         <v>100</v>
       </c>
-      <c s="31" r="U56"/>
+      <c s="32" r="U56"/>
     </row>
     <row customHeight="1" r="57" ht="15.0">
-      <c s="18" r="A57">
+      <c s="19" r="A57">
         <v>56.0</v>
       </c>
-      <c t="s" s="49" r="B57">
+      <c t="s" s="50" r="B57">
         <v>237</v>
       </c>
-      <c s="25" r="E57"/>
-      <c t="str" s="24" r="F57">
+      <c s="26" r="E57"/>
+      <c t="str" s="25" r="F57">
         <f>960-SUM(F7:F56)</f>
         <v>103</v>
       </c>
-      <c t="s" s="24" r="G57">
+      <c t="s" s="25" r="G57">
         <v>238</v>
       </c>
-      <c s="50" r="H57"/>
-      <c s="50" r="I57"/>
-      <c s="50" r="J57"/>
-      <c t="s" s="51" r="K57">
+      <c s="51" r="H57"/>
+      <c s="51" r="I57"/>
+      <c s="51" r="J57"/>
+      <c t="s" s="52" r="K57">
         <v>239</v>
       </c>
-      <c t="s" s="51" r="L57">
+      <c t="s" s="52" r="L57">
         <v>240</v>
       </c>
-      <c s="50" r="M57">
+      <c s="51" r="M57">
         <v>14.0</v>
       </c>
-      <c s="50" r="N57">
+      <c s="51" r="N57">
         <v>14.0</v>
       </c>
-      <c s="50" r="O57">
+      <c s="51" r="O57">
         <v>15.0</v>
       </c>
-      <c s="50" r="P57">
+      <c s="51" r="P57">
         <v>15.0</v>
       </c>
-      <c s="50" r="Q57">
+      <c s="51" r="Q57">
         <v>15.0</v>
       </c>
-      <c s="50" r="R57">
+      <c s="51" r="R57">
         <v>15.0</v>
       </c>
-      <c s="50" r="S57">
+      <c s="51" r="S57">
         <v>15.0</v>
       </c>
-      <c t="str" s="31" r="T57">
+      <c t="str" s="32" r="T57">
         <f>SUM(H57:S57)</f>
         <v>103</v>
       </c>
-      <c s="31" r="U57"/>
+      <c s="32" r="U57"/>
     </row>
     <row r="58">
-      <c t="s" s="18" r="A58">
+      <c t="s" s="19" r="A58">
         <v>241</v>
       </c>
-      <c t="s" s="49" r="B58">
+      <c t="s" s="50" r="B58">
         <v>242</v>
       </c>
-      <c t="s" s="25" r="E58">
+      <c t="s" s="26" r="E58">
         <v>243</v>
       </c>
-      <c s="24" r="F58"/>
-      <c s="52" r="G58"/>
-      <c s="50" r="H58"/>
-      <c s="50" r="I58"/>
-      <c s="50" r="J58"/>
-      <c t="s" s="53" r="K58">
+      <c s="25" r="F58"/>
+      <c s="53" r="G58"/>
+      <c s="51" r="H58"/>
+      <c s="51" r="I58"/>
+      <c s="51" r="J58"/>
+      <c t="s" s="54" r="K58">
         <v>244</v>
       </c>
-      <c t="s" s="53" r="L58">
+      <c t="s" s="54" r="L58">
         <v>245</v>
       </c>
-      <c s="50" r="M58"/>
-      <c t="s" s="50" r="N58">
+      <c s="51" r="M58"/>
+      <c t="s" s="51" r="N58">
         <v>246</v>
       </c>
-      <c s="50" r="O58"/>
-      <c s="50" r="P58"/>
-      <c s="50" r="Q58"/>
-      <c s="50" r="R58"/>
-      <c s="54" r="S58"/>
-      <c t="str" s="30" r="T58">
+      <c s="51" r="O58"/>
+      <c s="51" r="P58"/>
+      <c s="51" r="Q58"/>
+      <c s="51" r="R58"/>
+      <c s="55" r="S58"/>
+      <c t="str" s="31" r="T58">
         <f>SUM(H58:S58)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U58"/>
+      <c s="32" r="U58"/>
     </row>
     <row r="59">
-      <c t="s" s="18" r="A59">
+      <c t="s" s="19" r="A59">
         <v>247</v>
       </c>
-      <c t="s" s="49" r="B59">
+      <c t="s" s="50" r="B59">
         <v>248</v>
       </c>
-      <c t="s" s="25" r="E59">
+      <c t="s" s="26" r="E59">
         <v>249</v>
       </c>
-      <c s="24" r="F59"/>
-      <c s="52" r="G59"/>
-      <c s="50" r="H59"/>
-      <c s="50" r="I59"/>
-      <c s="50" r="J59"/>
-      <c t="s" s="29" r="K59">
+      <c s="25" r="F59"/>
+      <c s="53" r="G59"/>
+      <c s="51" r="H59"/>
+      <c s="51" r="I59"/>
+      <c s="51" r="J59"/>
+      <c t="s" s="30" r="K59">
         <v>250</v>
       </c>
-      <c t="s" s="29" r="L59">
+      <c t="s" s="30" r="L59">
         <v>251</v>
       </c>
-      <c s="50" r="M59"/>
-      <c s="50" r="N59"/>
-      <c t="s" s="50" r="O59">
+      <c s="51" r="M59"/>
+      <c s="51" r="N59"/>
+      <c t="s" s="51" r="O59">
         <v>252</v>
       </c>
-      <c s="50" r="P59"/>
-      <c s="50" r="Q59"/>
-      <c s="50" r="R59"/>
-      <c s="54" r="S59"/>
-      <c t="str" s="33" r="T59">
+      <c s="51" r="P59"/>
+      <c s="51" r="Q59"/>
+      <c s="51" r="R59"/>
+      <c s="55" r="S59"/>
+      <c t="str" s="34" r="T59">
         <f>SUM(H59:S59)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U59"/>
+      <c s="32" r="U59"/>
     </row>
     <row r="60">
-      <c t="s" s="18" r="A60">
+      <c t="s" s="19" r="A60">
         <v>253</v>
       </c>
-      <c t="s" s="49" r="B60">
+      <c t="s" s="50" r="B60">
         <v>254</v>
       </c>
-      <c t="s" s="25" r="E60">
+      <c t="s" s="26" r="E60">
         <v>255</v>
       </c>
-      <c s="24" r="F60"/>
-      <c s="52" r="G60"/>
-      <c s="50" r="H60"/>
-      <c s="50" r="I60"/>
-      <c s="50" r="J60"/>
-      <c t="s" s="29" r="K60">
+      <c s="25" r="F60"/>
+      <c s="53" r="G60"/>
+      <c s="51" r="H60"/>
+      <c s="51" r="I60"/>
+      <c s="51" r="J60"/>
+      <c t="s" s="30" r="K60">
         <v>256</v>
       </c>
-      <c t="s" s="29" r="L60">
+      <c t="s" s="30" r="L60">
         <v>257</v>
       </c>
-      <c s="50" r="M60"/>
-      <c s="50" r="N60"/>
-      <c t="s" s="50" r="O60">
+      <c s="51" r="M60"/>
+      <c s="51" r="N60"/>
+      <c t="s" s="51" r="O60">
         <v>258</v>
       </c>
-      <c s="50" r="P60"/>
-      <c s="50" r="Q60"/>
-      <c s="50" r="R60"/>
-      <c s="54" r="S60"/>
-      <c t="str" s="33" r="T60">
+      <c s="51" r="P60"/>
+      <c s="51" r="Q60"/>
+      <c s="51" r="R60"/>
+      <c s="55" r="S60"/>
+      <c t="str" s="34" r="T60">
         <f>SUM(H60:S60)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U60"/>
+      <c s="32" r="U60"/>
     </row>
     <row r="61">
-      <c t="s" s="18" r="A61">
+      <c t="s" s="19" r="A61">
         <v>259</v>
       </c>
-      <c t="s" s="49" r="B61">
+      <c t="s" s="50" r="B61">
         <v>260</v>
       </c>
-      <c t="s" s="25" r="E61">
+      <c t="s" s="26" r="E61">
         <v>261</v>
       </c>
-      <c s="24" r="F61"/>
-      <c s="52" r="G61"/>
-      <c s="50" r="H61"/>
-      <c s="50" r="I61"/>
-      <c s="50" r="J61"/>
-      <c t="s" s="29" r="K61">
+      <c s="25" r="F61"/>
+      <c s="53" r="G61"/>
+      <c s="51" r="H61"/>
+      <c s="51" r="I61"/>
+      <c s="51" r="J61"/>
+      <c t="s" s="30" r="K61">
         <v>262</v>
       </c>
-      <c t="s" s="29" r="L61">
+      <c t="s" s="30" r="L61">
         <v>263</v>
       </c>
-      <c s="50" r="M61"/>
-      <c s="50" r="N61"/>
-      <c s="50" r="O61"/>
-      <c t="s" s="50" r="P61">
+      <c s="51" r="M61"/>
+      <c s="51" r="N61"/>
+      <c s="51" r="O61"/>
+      <c t="s" s="51" r="P61">
         <v>264</v>
       </c>
-      <c s="50" r="Q61"/>
-      <c s="50" r="R61"/>
-      <c s="54" r="S61"/>
-      <c t="str" s="33" r="T61">
+      <c s="51" r="Q61"/>
+      <c s="51" r="R61"/>
+      <c s="55" r="S61"/>
+      <c t="str" s="34" r="T61">
         <f>SUM(H61:S61)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U61"/>
+      <c s="32" r="U61"/>
     </row>
     <row r="62">
-      <c t="s" s="18" r="A62">
+      <c t="s" s="19" r="A62">
         <v>265</v>
       </c>
-      <c t="s" s="49" r="B62">
+      <c t="s" s="50" r="B62">
         <v>266</v>
       </c>
-      <c t="s" s="25" r="E62">
+      <c t="s" s="26" r="E62">
         <v>267</v>
       </c>
-      <c s="24" r="F62"/>
-      <c s="52" r="G62"/>
-      <c s="50" r="H62"/>
-      <c s="50" r="I62"/>
-      <c s="50" r="J62"/>
-      <c t="s" s="29" r="K62">
+      <c s="25" r="F62"/>
+      <c s="53" r="G62"/>
+      <c s="51" r="H62"/>
+      <c s="51" r="I62"/>
+      <c s="51" r="J62"/>
+      <c t="s" s="30" r="K62">
         <v>268</v>
       </c>
-      <c t="s" s="29" r="L62">
+      <c t="s" s="30" r="L62">
         <v>269</v>
       </c>
-      <c s="50" r="M62"/>
-      <c s="50" r="N62"/>
-      <c s="50" r="O62"/>
-      <c s="50" r="P62"/>
-      <c t="s" s="50" r="Q62">
+      <c s="51" r="M62"/>
+      <c s="51" r="N62"/>
+      <c s="51" r="O62"/>
+      <c s="51" r="P62"/>
+      <c t="s" s="51" r="Q62">
         <v>270</v>
       </c>
-      <c s="52" r="R62"/>
-      <c s="50" r="S62"/>
-      <c t="str" s="55" r="T62">
+      <c s="53" r="R62"/>
+      <c s="51" r="S62"/>
+      <c t="str" s="56" r="T62">
         <f>SUM(H62:S62)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U62"/>
+      <c s="32" r="U62"/>
     </row>
     <row r="63">
-      <c t="s" s="18" r="A63">
+      <c t="s" s="19" r="A63">
         <v>271</v>
       </c>
-      <c t="s" s="49" r="B63">
+      <c t="s" s="50" r="B63">
         <v>272</v>
       </c>
-      <c t="s" s="25" r="E63">
+      <c t="s" s="26" r="E63">
         <v>273</v>
       </c>
-      <c s="24" r="F63"/>
-      <c s="52" r="G63"/>
-      <c s="50" r="H63"/>
-      <c s="50" r="I63"/>
-      <c s="50" r="J63"/>
-      <c t="s" s="29" r="K63">
+      <c s="25" r="F63"/>
+      <c s="53" r="G63"/>
+      <c s="51" r="H63"/>
+      <c s="51" r="I63"/>
+      <c s="51" r="J63"/>
+      <c t="s" s="30" r="K63">
         <v>274</v>
       </c>
-      <c t="s" s="29" r="L63">
+      <c t="s" s="30" r="L63">
         <v>275</v>
       </c>
-      <c s="50" r="M63"/>
-      <c s="50" r="N63"/>
-      <c s="50" r="O63"/>
-      <c s="50" r="P63"/>
-      <c s="50" r="Q63"/>
-      <c t="s" s="50" r="R63">
+      <c s="51" r="M63"/>
+      <c s="51" r="N63"/>
+      <c s="51" r="O63"/>
+      <c s="51" r="P63"/>
+      <c s="51" r="Q63"/>
+      <c t="s" s="51" r="R63">
         <v>276</v>
       </c>
-      <c s="54" r="S63"/>
-      <c t="str" s="33" r="T63">
+      <c s="55" r="S63"/>
+      <c t="str" s="34" r="T63">
         <f>SUM(H63:S63)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U63"/>
+      <c s="32" r="U63"/>
     </row>
     <row customHeight="1" r="64" ht="1.5">
-      <c t="s" s="18" r="A64">
+      <c t="s" s="19" r="A64">
         <v>277</v>
       </c>
-      <c t="s" s="49" r="B64">
+      <c t="s" s="50" r="B64">
         <v>278</v>
       </c>
-      <c s="25" r="E64"/>
-      <c s="24" r="F64"/>
-      <c s="52" r="G64"/>
-      <c s="50" r="H64"/>
-      <c s="50" r="I64"/>
-      <c s="50" r="J64"/>
-      <c t="s" s="29" r="K64">
+      <c s="26" r="E64"/>
+      <c s="25" r="F64"/>
+      <c s="53" r="G64"/>
+      <c s="51" r="H64"/>
+      <c s="51" r="I64"/>
+      <c s="51" r="J64"/>
+      <c t="s" s="30" r="K64">
         <v>279</v>
       </c>
-      <c t="s" s="29" r="L64">
+      <c t="s" s="30" r="L64">
         <v>280</v>
       </c>
-      <c s="50" r="M64"/>
-      <c s="50" r="N64"/>
-      <c s="50" r="O64"/>
-      <c s="50" r="P64"/>
-      <c s="50" r="Q64"/>
-      <c s="50" r="R64"/>
-      <c t="s" s="54" r="S64">
+      <c s="51" r="M64"/>
+      <c s="51" r="N64"/>
+      <c s="51" r="O64"/>
+      <c s="51" r="P64"/>
+      <c s="51" r="Q64"/>
+      <c s="51" r="R64"/>
+      <c t="s" s="55" r="S64">
         <v>281</v>
       </c>
-      <c t="str" s="31" r="T64">
+      <c t="str" s="32" r="T64">
         <f>SUM(H64:S64)</f>
         <v>0</v>
       </c>
-      <c s="31" r="U64"/>
+      <c s="32" r="U64"/>
     </row>
     <row r="65">
-      <c t="s" s="18" r="A65">
+      <c t="s" s="19" r="A65">
         <v>282</v>
       </c>
-      <c t="s" s="49" r="B65">
+      <c t="s" s="50" r="B65">
         <v>283</v>
       </c>
-      <c s="25" r="E65"/>
-      <c s="24" r="F65"/>
-      <c s="52" r="G65"/>
-      <c t="s" s="56" r="H65">
+      <c s="26" r="E65"/>
+      <c s="25" r="F65"/>
+      <c s="53" r="G65"/>
+      <c t="s" s="57" r="H65">
         <v>284</v>
       </c>
-      <c s="50" r="I65"/>
-      <c s="50" r="J65"/>
-      <c t="s" s="29" r="K65">
+      <c s="51" r="I65"/>
+      <c s="51" r="J65"/>
+      <c t="s" s="30" r="K65">
         <v>285</v>
       </c>
-      <c t="s" s="29" r="L65">
+      <c t="s" s="30" r="L65">
         <v>286</v>
       </c>
-      <c s="50" r="M65"/>
-      <c s="50" r="N65"/>
-      <c s="50" r="O65"/>
-      <c s="50" r="P65"/>
-      <c s="50" r="Q65"/>
-      <c s="50" r="R65"/>
-      <c s="54" r="S65"/>
-      <c s="31" r="T65"/>
-      <c s="31" r="U65"/>
+      <c s="51" r="M65"/>
+      <c s="51" r="N65"/>
+      <c s="51" r="O65"/>
+      <c s="51" r="P65"/>
+      <c s="51" r="Q65"/>
+      <c s="51" r="R65"/>
+      <c s="55" r="S65"/>
+      <c s="32" r="T65"/>
+      <c s="32" r="U65"/>
     </row>
     <row r="66">
-      <c t="s" s="18" r="A66">
+      <c t="s" s="19" r="A66">
         <v>287</v>
       </c>
-      <c t="s" s="49" r="B66">
+      <c t="s" s="50" r="B66">
         <v>288</v>
       </c>
-      <c s="25" r="E66"/>
-      <c s="24" r="F66"/>
-      <c s="52" r="G66"/>
-      <c s="50" r="H66"/>
-      <c s="50" r="I66"/>
-      <c s="50" r="J66"/>
-      <c t="s" s="29" r="K66">
+      <c s="26" r="E66"/>
+      <c s="25" r="F66"/>
+      <c s="53" r="G66"/>
+      <c s="51" r="H66"/>
+      <c s="51" r="I66"/>
+      <c s="51" r="J66"/>
+      <c t="s" s="30" r="K66">
         <v>289</v>
       </c>
-      <c t="s" s="29" r="L66">
+      <c t="s" s="30" r="L66">
         <v>290</v>
       </c>
-      <c t="s" s="56" r="M66">
+      <c t="s" s="57" r="M66">
         <v>291</v>
       </c>
-      <c s="50" r="N66"/>
-      <c s="50" r="O66"/>
-      <c s="50" r="P66"/>
-      <c s="50" r="Q66"/>
-      <c s="50" r="R66"/>
-      <c s="54" r="S66"/>
-      <c s="31" r="T66"/>
-      <c s="31" r="U66"/>
+      <c s="51" r="N66"/>
+      <c s="51" r="O66"/>
+      <c s="51" r="P66"/>
+      <c s="51" r="Q66"/>
+      <c s="51" r="R66"/>
+      <c s="55" r="S66"/>
+      <c s="32" r="T66"/>
+      <c s="32" r="U66"/>
     </row>
     <row r="67">
-      <c t="s" s="18" r="A67">
+      <c t="s" s="19" r="A67">
         <v>292</v>
       </c>
-      <c t="s" s="49" r="B67">
+      <c t="s" s="50" r="B67">
         <v>293</v>
       </c>
-      <c s="25" r="E67"/>
-      <c s="24" r="F67"/>
-      <c s="52" r="G67"/>
-      <c s="50" r="H67"/>
-      <c s="50" r="I67"/>
-      <c s="50" r="J67"/>
-      <c t="s" s="29" r="K67">
+      <c s="26" r="E67"/>
+      <c s="25" r="F67"/>
+      <c s="53" r="G67"/>
+      <c s="51" r="H67"/>
+      <c s="51" r="I67"/>
+      <c s="51" r="J67"/>
+      <c t="s" s="30" r="K67">
         <v>294</v>
       </c>
-      <c t="s" s="29" r="L67">
+      <c t="s" s="30" r="L67">
         <v>295</v>
       </c>
-      <c s="50" r="M67"/>
-      <c s="50" r="N67"/>
-      <c s="50" r="O67"/>
-      <c s="50" r="P67"/>
-      <c s="50" r="Q67"/>
-      <c s="50" r="R67"/>
-      <c t="s" s="57" r="S67">
+      <c s="51" r="M67"/>
+      <c s="51" r="N67"/>
+      <c s="51" r="O67"/>
+      <c s="51" r="P67"/>
+      <c s="51" r="Q67"/>
+      <c s="51" r="R67"/>
+      <c t="s" s="58" r="S67">
         <v>296</v>
       </c>
-      <c s="31" r="T67"/>
-      <c s="31" r="U67"/>
+      <c s="32" r="T67"/>
+      <c s="32" r="U67"/>
     </row>
     <row r="68">
-      <c t="s" s="18" r="A68">
+      <c t="s" s="19" r="A68">
         <v>297</v>
       </c>
-      <c t="s" s="49" r="B68">
+      <c t="s" s="50" r="B68">
         <v>298</v>
       </c>
-      <c s="25" r="E68"/>
-      <c s="24" r="F68"/>
-      <c s="52" r="G68"/>
-      <c s="50" r="H68"/>
-      <c s="50" r="I68"/>
-      <c s="50" r="J68"/>
-      <c t="s" s="29" r="K68">
+      <c s="26" r="E68"/>
+      <c s="25" r="F68"/>
+      <c s="53" r="G68"/>
+      <c s="51" r="H68"/>
+      <c s="51" r="I68"/>
+      <c s="51" r="J68"/>
+      <c t="s" s="30" r="K68">
         <v>299</v>
       </c>
-      <c t="s" s="29" r="L68">
+      <c t="s" s="30" r="L68">
         <v>300</v>
       </c>
-      <c s="50" r="M68"/>
-      <c s="50" r="N68"/>
-      <c s="50" r="O68"/>
-      <c s="50" r="P68"/>
-      <c s="50" r="Q68"/>
-      <c s="50" r="R68"/>
-      <c t="s" s="57" r="S68">
+      <c s="51" r="M68"/>
+      <c s="51" r="N68"/>
+      <c s="51" r="O68"/>
+      <c s="51" r="P68"/>
+      <c s="51" r="Q68"/>
+      <c s="51" r="R68"/>
+      <c t="s" s="58" r="S68">
         <v>301</v>
       </c>
-      <c s="31" r="T68"/>
-      <c s="31" r="U68"/>
+      <c s="32" r="T68"/>
+      <c s="32" r="U68"/>
     </row>
     <row customHeight="1" r="69" ht="2.25">
-      <c t="s" s="58" r="A69">
+      <c t="s" s="59" r="A69">
         <v>302</v>
       </c>
-      <c t="s" s="59" r="B69">
+      <c t="s" s="60" r="B69">
         <v>303</v>
       </c>
-      <c s="19" r="E69"/>
-      <c t="str" s="18" r="F69">
+      <c s="20" r="E69"/>
+      <c t="str" s="19" r="F69">
         <f>SUM(F7:F57)</f>
         <v>960</v>
       </c>
-      <c s="60" r="G69"/>
-      <c t="str" s="31" r="H69">
+      <c s="61" r="G69"/>
+      <c t="str" s="32" r="H69">
         <f>SUM(H7:H64)</f>
         <v>34</v>
       </c>
-      <c t="str" s="31" r="I69">
+      <c t="str" s="32" r="I69">
         <f>SUM(I7:I64)</f>
         <v>35</v>
       </c>
-      <c t="str" s="31" r="J69">
+      <c t="str" s="32" r="J69">
         <f>SUM(J7:J64)</f>
         <v>34</v>
       </c>
-      <c t="str" s="31" r="K69">
+      <c t="str" s="32" r="K69">
         <f>SUM(K7:K64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="31" r="L69">
+      <c t="str" s="32" r="L69">
         <f>SUM(L7:L64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="31" r="M69">
+      <c t="str" s="32" r="M69">
         <f>SUM(M7:M64)</f>
         <v>122</v>
       </c>
-      <c t="str" s="31" r="N69">
+      <c t="str" s="32" r="N69">
         <f>SUM(N7:N64)</f>
         <v>122</v>
       </c>
-      <c t="str" s="31" r="O69">
+      <c t="str" s="32" r="O69">
         <f>SUM(O7:O64)</f>
         <v>123</v>
       </c>
-      <c t="str" s="31" r="P69">
+      <c t="str" s="32" r="P69">
         <f>SUM(P7:P64)</f>
         <v>143</v>
       </c>
-      <c t="str" s="31" r="Q69">
+      <c t="str" s="32" r="Q69">
         <f>SUM(Q7:Q64)</f>
         <v>129</v>
       </c>
-      <c t="str" s="31" r="R69">
+      <c t="str" s="32" r="R69">
         <f>SUM(R7:R64)</f>
         <v>110</v>
       </c>
-      <c t="str" s="31" r="S69">
+      <c t="str" s="32" r="S69">
         <f>SUM(S7:S64)</f>
         <v>108</v>
       </c>
-      <c t="str" s="31" r="T69">
+      <c t="str" s="32" r="T69">
         <f>SUM(H69:S69)</f>
         <v>960</v>
       </c>
-      <c s="31" r="U69"/>
+      <c s="32" r="U69"/>
     </row>
     <row r="70" hidden="1">
-      <c s="61" r="E70"/>
-      <c t="str" s="52" r="F70">
+      <c s="62" r="E70"/>
+      <c t="str" s="53" r="F70">
         <f>SUMIF($G$7:$G$64, $G70, F$7:F$64)</f>
         <v>64</v>
       </c>
-      <c t="s" s="24" r="G70">
+      <c t="s" s="25" r="G70">
         <v>304</v>
       </c>
-      <c t="str" s="52" r="H70">
+      <c t="str" s="53" r="H70">
         <f>SUMIF($G$7:$G$64, $G70, H$7:H$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="I70">
+      <c t="str" s="53" r="I70">
         <f>SUMIF($G$7:$G$64, $G70, I$7:I$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="J70">
+      <c t="str" s="53" r="J70">
         <f>SUMIF($G$7:$G$64, $G70, J$7:J$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="K70">
+      <c t="str" s="53" r="K70">
         <f>SUMIF($G$7:$G$64, $G70, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L70">
+      <c t="str" s="53" r="L70">
         <f>SUMIF($G$7:$G$64, $G70, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M70">
+      <c t="str" s="53" r="M70">
         <f>SUMIF($G$7:$G$64, $G70, M$7:M$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="N70">
+      <c t="str" s="53" r="N70">
         <f>SUMIF($G$7:$G$64, $G70, N$7:N$64)</f>
         <v>16</v>
       </c>
-      <c t="str" s="52" r="O70">
+      <c t="str" s="53" r="O70">
         <f>SUMIF($G$7:$G$64, $G70, O$7:O$64)</f>
         <v>8</v>
       </c>
-      <c t="str" s="52" r="P70">
+      <c t="str" s="53" r="P70">
         <f>SUMIF($G$7:$G$64, $G70, P$7:P$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="Q70">
+      <c t="str" s="53" r="Q70">
         <f>SUMIF($G$7:$G$64, $G70, Q$7:Q$64)</f>
         <v>16</v>
       </c>
-      <c t="str" s="52" r="R70">
+      <c t="str" s="53" r="R70">
         <f>SUMIF($G$7:$G$64, $G70, R$7:R$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="S70">
+      <c t="str" s="53" r="S70">
         <f>SUMIF($G$7:$G$64, $G70, S$7:S$64)</f>
         <v>0</v>
       </c>
-      <c s="52" r="U70"/>
+      <c s="53" r="U70"/>
     </row>
     <row r="71" hidden="1">
-      <c s="61" r="E71"/>
-      <c t="str" s="52" r="F71">
+      <c s="62" r="E71"/>
+      <c t="str" s="53" r="F71">
         <f>SUMIF($G$7:$G$64, $G71, F$7:F$64)</f>
         <v>46</v>
       </c>
-      <c t="s" s="24" r="G71">
+      <c t="s" s="25" r="G71">
         <v>305</v>
       </c>
-      <c t="str" s="52" r="H71">
+      <c t="str" s="53" r="H71">
         <f>SUMIF($G$7:$G$64, $G71, H$7:H$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="I71">
+      <c t="str" s="53" r="I71">
         <f>SUMIF($G$7:$G$64, $G71, I$7:I$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="J71">
+      <c t="str" s="53" r="J71">
         <f>SUMIF($G$7:$G$64, $G71, J$7:J$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="K71">
+      <c t="str" s="53" r="K71">
         <f>SUMIF($G$7:$G$64, $G71, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L71">
+      <c t="str" s="53" r="L71">
         <f>SUMIF($G$7:$G$64, $G71, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M71">
+      <c t="str" s="53" r="M71">
         <f>SUMIF($G$7:$G$64, $G71, M$7:M$64)</f>
         <v>22</v>
       </c>
-      <c t="str" s="52" r="N71">
+      <c t="str" s="53" r="N71">
         <f>SUMIF($G$7:$G$64, $G71, N$7:N$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="O71">
+      <c t="str" s="53" r="O71">
         <f>SUMIF($G$7:$G$64, $G71, O$7:O$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="P71">
+      <c t="str" s="53" r="P71">
         <f>SUMIF($G$7:$G$64, $G71, P$7:P$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="Q71">
+      <c t="str" s="53" r="Q71">
         <f>SUMIF($G$7:$G$64, $G71, Q$7:Q$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="R71">
+      <c t="str" s="53" r="R71">
         <f>SUMIF($G$7:$G$64, $G71, R$7:R$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="S71">
+      <c t="str" s="53" r="S71">
         <f>SUMIF($G$7:$G$64, $G71, S$7:S$64)</f>
         <v>0</v>
       </c>
-      <c s="52" r="U71"/>
+      <c s="53" r="U71"/>
     </row>
     <row r="72" hidden="1">
-      <c s="61" r="E72"/>
-      <c t="str" s="52" r="F72">
+      <c s="62" r="E72"/>
+      <c t="str" s="53" r="F72">
         <f>SUMIF($G$7:$G$64, $G72, F$7:F$64)</f>
         <v>116</v>
       </c>
-      <c t="s" s="24" r="G72">
+      <c t="s" s="25" r="G72">
         <v>306</v>
       </c>
-      <c t="str" s="52" r="H72">
+      <c t="str" s="53" r="H72">
         <f>SUMIF($G$7:$G$64, $G72, H$7:H$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="I72">
+      <c t="str" s="53" r="I72">
         <f>SUMIF($G$7:$G$64, $G72, I$7:I$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="J72">
+      <c t="str" s="53" r="J72">
         <f>SUMIF($G$7:$G$64, $G72, J$7:J$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="K72">
+      <c t="str" s="53" r="K72">
         <f>SUMIF($G$7:$G$64, $G72, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L72">
+      <c t="str" s="53" r="L72">
         <f>SUMIF($G$7:$G$64, $G72, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M72">
+      <c t="str" s="53" r="M72">
         <f>SUMIF($G$7:$G$64, $G72, M$7:M$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="N72">
+      <c t="str" s="53" r="N72">
         <f>SUMIF($G$7:$G$64, $G72, N$7:N$64)</f>
         <v>36</v>
       </c>
-      <c t="str" s="52" r="O72">
+      <c t="str" s="53" r="O72">
         <f>SUMIF($G$7:$G$64, $G72, O$7:O$64)</f>
         <v>32</v>
       </c>
-      <c t="str" s="52" r="P72">
+      <c t="str" s="53" r="P72">
         <f>SUMIF($G$7:$G$64, $G72, P$7:P$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="Q72">
+      <c t="str" s="53" r="Q72">
         <f>SUMIF($G$7:$G$64, $G72, Q$7:Q$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="R72">
+      <c t="str" s="53" r="R72">
         <f>SUMIF($G$7:$G$64, $G72, R$7:R$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="S72">
+      <c t="str" s="53" r="S72">
         <f>SUMIF($G$7:$G$64, $G72, S$7:S$64)</f>
         <v>0</v>
       </c>
-      <c s="52" r="U72"/>
+      <c s="53" r="U72"/>
     </row>
     <row r="73" hidden="1">
-      <c s="61" r="E73"/>
-      <c t="str" s="52" r="F73">
+      <c s="62" r="E73"/>
+      <c t="str" s="53" r="F73">
         <f>SUMIF($G$7:$G$64, $G73, F$7:F$64)</f>
         <v>72</v>
       </c>
-      <c t="s" s="24" r="G73">
+      <c t="s" s="25" r="G73">
         <v>307</v>
       </c>
-      <c t="str" s="52" r="H73">
+      <c t="str" s="53" r="H73">
         <f>SUMIF($G$7:$G$64, $G73, H$7:H$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="I73">
+      <c t="str" s="53" r="I73">
         <f>SUMIF($G$7:$G$64, $G73, I$7:I$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="J73">
+      <c t="str" s="53" r="J73">
         <f>SUMIF($G$7:$G$64, $G73, J$7:J$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="K73">
+      <c t="str" s="53" r="K73">
         <f>SUMIF($G$7:$G$64, $G73, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L73">
+      <c t="str" s="53" r="L73">
         <f>SUMIF($G$7:$G$64, $G73, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M73">
+      <c t="str" s="53" r="M73">
         <f>SUMIF($G$7:$G$64, $G73, M$7:M$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="N73">
+      <c t="str" s="53" r="N73">
         <f>SUMIF($G$7:$G$64, $G73, N$7:N$64)</f>
         <v>4</v>
       </c>
-      <c t="str" s="52" r="O73">
+      <c t="str" s="53" r="O73">
         <f>SUMIF($G$7:$G$64, $G73, O$7:O$64)</f>
         <v>40</v>
       </c>
-      <c t="str" s="52" r="P73">
+      <c t="str" s="53" r="P73">
         <f>SUMIF($G$7:$G$64, $G73, P$7:P$64)</f>
         <v>12</v>
       </c>
-      <c t="str" s="52" r="Q73">
+      <c t="str" s="53" r="Q73">
         <f>SUMIF($G$7:$G$64, $G73, Q$7:Q$64)</f>
         <v>8</v>
       </c>
-      <c t="str" s="52" r="R73">
+      <c t="str" s="53" r="R73">
         <f>SUMIF($G$7:$G$64, $G73, R$7:R$64)</f>
         <v>8</v>
       </c>
-      <c t="str" s="52" r="S73">
+      <c t="str" s="53" r="S73">
         <f>SUMIF($G$7:$G$64, $G73, S$7:S$64)</f>
         <v>0</v>
       </c>
-      <c s="52" r="U73"/>
+      <c s="53" r="U73"/>
     </row>
     <row r="74" hidden="1">
-      <c s="61" r="E74"/>
-      <c t="str" s="52" r="F74">
+      <c s="62" r="E74"/>
+      <c t="str" s="53" r="F74">
         <f>SUMIF($G$7:$G$64, $G74, F$7:F$64)</f>
         <v>114</v>
       </c>
-      <c t="s" s="24" r="G74">
+      <c t="s" s="25" r="G74">
         <v>308</v>
       </c>
-      <c t="str" s="52" r="H74">
+      <c t="str" s="53" r="H74">
         <f>SUMIF($G$7:$G$64, $G74, H$7:H$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="I74">
+      <c t="str" s="53" r="I74">
         <f>SUMIF($G$7:$G$64, $G74, I$7:I$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="J74">
+      <c t="str" s="53" r="J74">
         <f>SUMIF($G$7:$G$64, $G74, J$7:J$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="K74">
+      <c t="str" s="53" r="K74">
         <f>SUMIF($G$7:$G$64, $G74, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L74">
+      <c t="str" s="53" r="L74">
         <f>SUMIF($G$7:$G$64, $G74, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M74">
+      <c t="str" s="53" r="M74">
         <f>SUMIF($G$7:$G$64, $G74, M$7:M$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="N74">
+      <c t="str" s="53" r="N74">
         <f>SUMIF($G$7:$G$64, $G74, N$7:N$64)</f>
         <v>25</v>
       </c>
-      <c t="str" s="52" r="O74">
+      <c t="str" s="53" r="O74">
         <f>SUMIF($G$7:$G$64, $G74, O$7:O$64)</f>
         <v>17</v>
       </c>
-      <c t="str" s="52" r="P74">
+      <c t="str" s="53" r="P74">
         <f>SUMIF($G$7:$G$64, $G74, P$7:P$64)</f>
         <v>17</v>
       </c>
-      <c t="str" s="52" r="Q74">
+      <c t="str" s="53" r="Q74">
         <f>SUMIF($G$7:$G$64, $G74, Q$7:Q$64)</f>
         <v>17</v>
       </c>
-      <c t="str" s="52" r="R74">
+      <c t="str" s="53" r="R74">
         <f>SUMIF($G$7:$G$64, $G74, R$7:R$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="S74">
+      <c t="str" s="53" r="S74">
         <f>SUMIF($G$7:$G$64, $G74, S$7:S$64)</f>
         <v>33</v>
       </c>
-      <c s="52" r="U74"/>
+      <c s="53" r="U74"/>
     </row>
     <row r="75" hidden="1">
-      <c s="61" r="E75"/>
-      <c t="str" s="52" r="F75">
+      <c s="62" r="E75"/>
+      <c t="str" s="53" r="F75">
         <f>SUMIF($G$7:$G$64, $G75, F$7:F$64)</f>
         <v>79</v>
       </c>
-      <c t="s" s="24" r="G75">
+      <c t="s" s="25" r="G75">
         <v>309</v>
       </c>
-      <c t="str" s="52" r="H75">
+      <c t="str" s="53" r="H75">
         <f>SUMIF($G$7:$G$64, $G75, H$7:H$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="I75">
+      <c t="str" s="53" r="I75">
         <f>SUMIF($G$7:$G$64, $G75, I$7:I$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="J75">
+      <c t="str" s="53" r="J75">
         <f>SUMIF($G$7:$G$64, $G75, J$7:J$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="K75">
+      <c t="str" s="53" r="K75">
         <f>SUMIF($G$7:$G$64, $G75, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L75">
+      <c t="str" s="53" r="L75">
         <f>SUMIF($G$7:$G$64, $G75, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M75">
+      <c t="str" s="53" r="M75">
         <f>SUMIF($G$7:$G$64, $G75, M$7:M$64)</f>
         <v>9</v>
       </c>
-      <c t="str" s="52" r="N75">
+      <c t="str" s="53" r="N75">
         <f>SUMIF($G$7:$G$64, $G75, N$7:N$64)</f>
         <v>17</v>
       </c>
-      <c t="str" s="52" r="O75">
+      <c t="str" s="53" r="O75">
         <f>SUMIF($G$7:$G$64, $G75, O$7:O$64)</f>
         <v>1</v>
       </c>
-      <c t="str" s="52" r="P75">
+      <c t="str" s="53" r="P75">
         <f>SUMIF($G$7:$G$64, $G75, P$7:P$64)</f>
         <v>5</v>
       </c>
-      <c t="str" s="52" r="Q75">
+      <c t="str" s="53" r="Q75">
         <f>SUMIF($G$7:$G$64, $G75, Q$7:Q$64)</f>
         <v>11</v>
       </c>
-      <c t="str" s="52" r="R75">
+      <c t="str" s="53" r="R75">
         <f>SUMIF($G$7:$G$64, $G75, R$7:R$64)</f>
         <v>20</v>
       </c>
-      <c t="str" s="52" r="S75">
+      <c t="str" s="53" r="S75">
         <f>SUMIF($G$7:$G$64, $G75, S$7:S$64)</f>
         <v>16</v>
       </c>
-      <c s="52" r="U75"/>
+      <c s="53" r="U75"/>
     </row>
     <row r="76" hidden="1">
-      <c s="61" r="E76"/>
-      <c t="str" s="52" r="F76">
+      <c s="62" r="E76"/>
+      <c t="str" s="53" r="F76">
         <f>SUMIF($G$7:$G$64, $G76, F$7:F$64)</f>
         <v>275</v>
       </c>
-      <c t="s" s="24" r="G76">
+      <c t="s" s="25" r="G76">
         <v>310</v>
       </c>
-      <c t="str" s="52" r="H76">
+      <c t="str" s="53" r="H76">
         <f>SUMIF($G$7:$G$64, $G76, H$7:H$64)</f>
         <v>33</v>
       </c>
-      <c t="str" s="52" r="I76">
+      <c t="str" s="53" r="I76">
         <f>SUMIF($G$7:$G$64, $G76, I$7:I$64)</f>
         <v>34</v>
       </c>
-      <c t="str" s="52" r="J76">
+      <c t="str" s="53" r="J76">
         <f>SUMIF($G$7:$G$64, $G76, J$7:J$64)</f>
         <v>33</v>
       </c>
-      <c t="str" s="52" r="K76">
+      <c t="str" s="53" r="K76">
         <f>SUMIF($G$7:$G$64, $G76, K$7:K$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="L76">
+      <c t="str" s="53" r="L76">
         <f>SUMIF($G$7:$G$64, $G76, L$7:L$64)</f>
         <v>0</v>
       </c>
-      <c t="str" s="52" r="M76">
+      <c t="str" s="53" r="M76">
         <f>SUMIF($G$7:$G$64, $G76, M$7:M$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="N76">
+      <c t="str" s="53" r="N76">
         <f>SUMIF($G$7:$G$64, $G76, N$7:N$64)</f>
         <v>24</v>
       </c>
-      <c t="str" s="52" r="O76">
+      <c t="str" s="53" r="O76">
         <f>SUMIF($G$7:$G$64, $G76, O$7:O$64)</f>
         <v>25</v>
       </c>
-      <c t="str" s="52" r="P76">
+      <c t="str" s="53" r="P76">
         <f>SUMIF($G$7:$G$64, $G76, P$7:P$64)</f>
         <v>25</v>
       </c>
-      <c t="str" s="52" r="Q76">
+      <c t="str" s="53" r="Q76">
         <f>SUMIF($G$7:$G$64, $G76, Q$7:Q$64)</f>
         <v>25</v>
       </c>
-      <c t="str" s="52" r="R76">
+      <c t="str" s="53" r="R76">
         <f>SUMIF($G$7:$G$64, $G76, R$7:R$64)</f>
         <v>25</v>
       </c>
-      <c t="str" s="52" r="S76">
+      <c t="str" s="53" r="S76">
         <f>SUMIF($G$7:$G$64, $G76, S$7:S$64)</f>
         <v>27</v>
       </c>
-      <c s="52" r="U76"/>
+      <c s="53" r="U76"/>
     </row>
     <row r="77" hidden="1">
-      <c s="61" r="E77"/>
-      <c t="str" s="62" r="F77">
+      <c s="62" r="E77"/>
+      <c t="str" s="63" r="F77">
         <f>SUM(F70:F76)</f>
         <v>766</v>
       </c>
-      <c t="str" s="62" r="G77">
+      <c t="str" s="63" r="G77">
         <f>SUM(G70:G76)</f>
         <v>0</v>
       </c>
-      <c t="str" s="62" r="H77">
+      <c t="str" s="63" r="H77">
         <f>SUM(H70:H76)</f>
         <v>34</v>
       </c>
-      <c t="str" s="62" r="I77">
+      <c t="str" s="63" r="I77">
         <f>SUM(I70:I76)</f>
         <v>35</v>
       </c>
-      <c t="str" s="62" r="J77">
+      <c t="str" s="63" r="J77">
         <f>SUM(J70:J76)</f>
         <v>34</v>
       </c>
-      <c t="str" s="62" r="K77">
+      <c t="str" s="63" r="K77">
         <f>SUM(K70:K76)</f>
         <v>0</v>
       </c>
-      <c t="str" s="62" r="L77">
+      <c t="str" s="63" r="L77">
         <f>SUM(L70:L76)</f>
         <v>0</v>
       </c>
-      <c t="str" s="62" r="M77">
+      <c t="str" s="63" r="M77">
         <f>SUM(M70:M76)</f>
         <v>80</v>
       </c>
-      <c t="str" s="62" r="N77">
+      <c t="str" s="63" r="N77">
         <f>SUM(N70:N76)</f>
         <v>122</v>
       </c>
-      <c t="str" s="62" r="O77">
+      <c t="str" s="63" r="O77">
         <f>SUM(O70:O76)</f>
         <v>123</v>
       </c>
-      <c t="str" s="62" r="P77">
+      <c t="str" s="63" r="P77">
         <f>SUM(P70:P76)</f>
         <v>83</v>
       </c>
-      <c t="str" s="62" r="Q77">
+      <c t="str" s="63" r="Q77">
         <f>SUM(Q70:Q76)</f>
         <v>101</v>
       </c>
-      <c t="str" s="62" r="R77">
+      <c t="str" s="63" r="R77">
         <f>SUM(R70:R76)</f>
         <v>78</v>
       </c>
-      <c t="str" s="62" r="S77">
+      <c t="str" s="63" r="S77">
         <f>SUM(S70:S76)</f>
         <v>76</v>
       </c>
-      <c s="52" r="U77"/>
+      <c s="53" r="U77"/>
     </row>
   </sheetData>
   <mergeCells count="82">

</xml_diff>